<commit_message>
Content - Rate and content setup for improved eggs
Former-commit-id: bdbdb0ff404c167d59eb57ec06780e168ec4104f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gatcha.xlsx
+++ b/Docs/Content/HungryDragonContent_Gatcha.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="88">
   <si>
     <t>dynamicGatcha</t>
   </si>
@@ -225,6 +225,69 @@
   </si>
   <si>
     <t>EGG DEFINITIONS</t>
+  </si>
+  <si>
+    <t>egg_rareGuaranteed</t>
+  </si>
+  <si>
+    <t>egg_epicGuaranteed</t>
+  </si>
+  <si>
+    <t>egg_betterRates</t>
+  </si>
+  <si>
+    <t>[weightCommon]</t>
+  </si>
+  <si>
+    <t>[weightRare]</t>
+  </si>
+  <si>
+    <t>[weightEpic]</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>3.8</t>
+  </si>
+  <si>
+    <t>PF_EggRareGuaranteed</t>
+  </si>
+  <si>
+    <t>PF_EggEpicGuaranteed</t>
+  </si>
+  <si>
+    <t>PF_EggBetterRates</t>
+  </si>
+  <si>
+    <t>TID_EGG_RARE</t>
+  </si>
+  <si>
+    <t>TID_EGG_EPIC</t>
+  </si>
+  <si>
+    <t>TID_EGG_BETTER</t>
+  </si>
+  <si>
+    <t>icon_egg_rare</t>
+  </si>
+  <si>
+    <t>icon_egg_epic</t>
+  </si>
+  <si>
+    <t>icon_egg_better</t>
+  </si>
+  <si>
+    <t>egg_rare</t>
+  </si>
+  <si>
+    <t>egg_epic</t>
+  </si>
+  <si>
+    <t>egg_better</t>
   </si>
 </sst>
 </file>
@@ -532,7 +595,82 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="48">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -752,13 +890,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -768,6 +899,13 @@
         <top style="thin">
           <color auto="1"/>
         </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -876,13 +1014,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -892,6 +1023,13 @@
         <top style="thin">
           <color auto="1"/>
         </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -1094,13 +1232,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -1110,6 +1241,13 @@
         <top style="thin">
           <color auto="1"/>
         </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -1306,13 +1444,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -1322,6 +1453,13 @@
         <top style="thin">
           <color auto="1"/>
         </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -1354,15 +1492,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="eggDefinitions" displayName="eggDefinitions" ref="B4:I9" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="42" tableBorderDxfId="43" totalsRowBorderDxfId="41">
-  <autoFilter ref="B4:I9"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="{eggDefinitions}" dataDxfId="40"/>
-    <tableColumn id="6" name="[sku]" dataDxfId="39"/>
-    <tableColumn id="4" name="[pricePC]" dataDxfId="38"/>
-    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="37"/>
-    <tableColumn id="10" name="[prefabPath]" dataDxfId="36"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="eggDefinitions" displayName="eggDefinitions" ref="B4:L12" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+  <autoFilter ref="B4:L12"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="{eggDefinitions}" dataDxfId="43"/>
+    <tableColumn id="6" name="[sku]" dataDxfId="42"/>
+    <tableColumn id="4" name="[pricePC]" dataDxfId="41"/>
+    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="40"/>
+    <tableColumn id="8" name="[weightCommon]" dataDxfId="2"/>
+    <tableColumn id="9" name="[weightRare]" dataDxfId="1"/>
+    <tableColumn id="11" name="[weightEpic]" dataDxfId="0"/>
+    <tableColumn id="10" name="[prefabPath]" dataDxfId="39"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="38"/>
     <tableColumn id="2" name="[icon]"/>
     <tableColumn id="3" name="[trackingSku]"/>
   </tableColumns>
@@ -1371,43 +1512,43 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="eggRewardDefinitions" displayName="eggRewardDefinitions" ref="B21:I25" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="32" tableBorderDxfId="33" totalsRowBorderDxfId="31">
-  <autoFilter ref="B21:I25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="eggRewardDefinitions" displayName="eggRewardDefinitions" ref="B23:I27" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="B23:I27"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="30"/>
+    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="33"/>
     <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[type]" dataDxfId="29"/>
-    <tableColumn id="6" name="[rarity]" dataDxfId="28"/>
-    <tableColumn id="4" name="[droprate]" dataDxfId="27"/>
-    <tableColumn id="7" name="[duplicateFragmentsGiven]" dataDxfId="26"/>
-    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="25"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="24"/>
+    <tableColumn id="3" name="[type]" dataDxfId="32"/>
+    <tableColumn id="6" name="[rarity]" dataDxfId="31"/>
+    <tableColumn id="4" name="[droprate]" dataDxfId="30"/>
+    <tableColumn id="7" name="[duplicateFragmentsGiven]" dataDxfId="29"/>
+    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="28"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="rarityDefinitions" displayName="rarityDefinitions" ref="B29:E33" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="21" tableBorderDxfId="22" totalsRowBorderDxfId="20">
-  <autoFilter ref="B29:E33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="rarityDefinitions" displayName="rarityDefinitions" ref="B31:E35" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+  <autoFilter ref="B31:E35"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="19"/>
+    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="22"/>
     <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[order]" dataDxfId="18"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="17"/>
+    <tableColumn id="3" name="[order]" dataDxfId="21"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="eggDefinitions26" displayName="eggDefinitions26" ref="B14:E17" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
-  <autoFilter ref="B14:E17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="eggDefinitions26" displayName="eggDefinitions26" ref="B16:E19" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+  <autoFilter ref="B16:E19"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{goldenEggDefinitions}" dataDxfId="12"/>
-    <tableColumn id="6" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="4" name="[order]" dataDxfId="10"/>
-    <tableColumn id="5" name="[fragmentsRequired]" dataDxfId="9"/>
+    <tableColumn id="1" name="{goldenEggDefinitions}" dataDxfId="15"/>
+    <tableColumn id="6" name="[sku]" dataDxfId="14"/>
+    <tableColumn id="4" name="[order]" dataDxfId="13"/>
+    <tableColumn id="5" name="[fragmentsRequired]" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1679,10 +1820,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="B1:Y38"/>
+  <dimension ref="B1:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1750,16 +1891,25 @@
       <c r="E4" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="J4" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="K4" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="37" t="s">
+      <c r="L4" s="37" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1776,16 +1926,25 @@
       <c r="E5" s="29">
         <v>360</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="20">
+        <v>1</v>
+      </c>
+      <c r="G5" s="20">
+        <v>2</v>
+      </c>
+      <c r="H5" s="20">
+        <v>3</v>
+      </c>
+      <c r="I5" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="J5" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="H5" t="s">
+      <c r="K5" t="s">
         <v>57</v>
       </c>
-      <c r="I5" t="s">
+      <c r="L5" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1802,16 +1961,25 @@
       <c r="E6" s="29">
         <v>0</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="20">
+        <v>1</v>
+      </c>
+      <c r="G6" s="20">
+        <v>2</v>
+      </c>
+      <c r="H6" s="20">
+        <v>3</v>
+      </c>
+      <c r="I6" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="36" t="s">
+      <c r="J6" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="H6" t="s">
+      <c r="K6" t="s">
         <v>47</v>
       </c>
-      <c r="I6" t="s">
+      <c r="L6" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1828,16 +1996,25 @@
       <c r="E7" s="29">
         <v>0</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="20">
+        <v>1</v>
+      </c>
+      <c r="G7" s="20">
+        <v>2</v>
+      </c>
+      <c r="H7" s="20">
+        <v>3</v>
+      </c>
+      <c r="I7" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="J7" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="H7" t="s">
+      <c r="K7" t="s">
         <v>52</v>
       </c>
-      <c r="I7" t="s">
+      <c r="L7" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1854,16 +2031,25 @@
       <c r="E8" s="33">
         <v>0</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="20">
+        <v>1</v>
+      </c>
+      <c r="G8" s="20">
+        <v>2</v>
+      </c>
+      <c r="H8" s="20">
+        <v>3</v>
+      </c>
+      <c r="I8" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="J8" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="K8" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="I8" s="26" t="s">
+      <c r="L8" s="26" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1880,81 +2066,163 @@
       <c r="E9" s="29">
         <v>0</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="20">
+        <v>1</v>
+      </c>
+      <c r="G9" s="20">
+        <v>2</v>
+      </c>
+      <c r="H9" s="20">
+        <v>3</v>
+      </c>
+      <c r="I9" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="J9" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="26" t="s">
+      <c r="K9" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="26" t="s">
-        <v>46</v>
+      <c r="L9" s="26" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-    </row>
-    <row r="11" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="2:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B12" s="8" t="s">
+      <c r="B10" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="20">
+        <v>0</v>
+      </c>
+      <c r="E10" s="29">
+        <v>0</v>
+      </c>
+      <c r="F10" s="29">
+        <v>0</v>
+      </c>
+      <c r="G10" s="29">
+        <v>2</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="L10" s="26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="20">
+        <v>0</v>
+      </c>
+      <c r="E11" s="29">
+        <v>0</v>
+      </c>
+      <c r="F11" s="29">
+        <v>0</v>
+      </c>
+      <c r="G11" s="29">
+        <v>0</v>
+      </c>
+      <c r="H11" s="29">
+        <v>1</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="J11" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="L11" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="20">
+        <v>0</v>
+      </c>
+      <c r="E12" s="29">
+        <v>0</v>
+      </c>
+      <c r="F12" s="29">
+        <v>1</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="J12" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="K12" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="L12" s="26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:25" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B14" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-    </row>
-    <row r="14" spans="2:25" ht="114" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="2:25" ht="114" x14ac:dyDescent="0.25">
+      <c r="B16" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C16" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D16" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E16" s="24" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="21">
-        <v>0</v>
-      </c>
-      <c r="E15" s="21">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="21">
-        <v>1</v>
-      </c>
-      <c r="E16" s="21">
-        <v>100</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -1962,122 +2230,98 @@
         <v>1</v>
       </c>
       <c r="C17" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="21">
+        <v>0</v>
+      </c>
+      <c r="E17" s="21">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="21">
+        <v>1</v>
+      </c>
+      <c r="E18" s="21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D19" s="21">
         <v>2</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E19" s="21">
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-    </row>
-    <row r="19" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B19" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-    </row>
-    <row r="20" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="17"/>
+    </row>
+    <row r="21" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B21" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+    </row>
+    <row r="22" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H22" s="18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="131.25" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
+    <row r="23" spans="2:9" ht="131.25" x14ac:dyDescent="0.25">
+      <c r="B23" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C23" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="D23" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E23" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F23" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="22" t="s">
+      <c r="G23" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="H21" s="22" t="s">
+      <c r="H23" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="I23" s="13" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="20">
-        <v>1</v>
-      </c>
-      <c r="G22" s="19">
-        <v>1</v>
-      </c>
-      <c r="H22" s="19">
-        <v>100</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="20">
-        <v>2</v>
-      </c>
-      <c r="G23" s="19">
-        <v>3</v>
-      </c>
-      <c r="H23" s="19">
-        <v>300</v>
-      </c>
-      <c r="I23" s="9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -2085,25 +2329,25 @@
         <v>1</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D24" s="21" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F24" s="20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G24" s="19">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H24" s="19">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
@@ -2111,88 +2355,112 @@
         <v>1</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>23</v>
       </c>
       <c r="E25" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="20">
+        <v>2</v>
+      </c>
+      <c r="G25" s="19">
+        <v>3</v>
+      </c>
+      <c r="H25" s="19">
+        <v>300</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="20">
+        <v>3</v>
+      </c>
+      <c r="G26" s="19">
+        <v>5</v>
+      </c>
+      <c r="H26" s="19">
+        <v>500</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="20">
+      <c r="F27" s="20">
         <v>0</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G27" s="19">
         <v>0</v>
       </c>
-      <c r="H25" s="19">
+      <c r="H27" s="19">
         <v>0</v>
       </c>
-      <c r="I25" s="9" t="s">
+      <c r="I27" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B27" s="8" t="s">
+    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B29" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="18" t="s">
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-    </row>
-    <row r="29" spans="2:9" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B29" s="16" t="s">
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+    </row>
+    <row r="31" spans="2:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="B31" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C31" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D31" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="E31" s="13" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="10">
-        <v>0</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="10">
-        <v>1</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
@@ -2200,13 +2468,13 @@
         <v>1</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D32" s="10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
@@ -2214,104 +2482,132 @@
         <v>1</v>
       </c>
       <c r="C33" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="10">
+        <v>1</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="10">
+        <v>2</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D35" s="10">
         <v>3</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E35" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B35" s="8" t="s">
+    <row r="36" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B37" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-    </row>
-    <row r="37" spans="2:7" ht="131.25" x14ac:dyDescent="0.25">
-      <c r="B37" s="7" t="s">
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+    </row>
+    <row r="39" spans="2:7" ht="131.25" x14ac:dyDescent="0.25">
+      <c r="B39" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C39" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D39" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E39" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F39" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="G39" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C38" s="3" t="s">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="2">
-        <v>1</v>
-      </c>
-      <c r="E38" s="1">
+      <c r="D40" s="2">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1">
         <v>4</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F40" s="1">
         <v>0.01</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G40" s="1">
         <v>1.4</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C22">
-    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="duplicateValues" dxfId="11" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23:C25">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+  <conditionalFormatting sqref="C25:C27">
+    <cfRule type="duplicateValues" dxfId="10" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:D30">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+  <conditionalFormatting sqref="C32:D32">
+    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31:D32">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+  <conditionalFormatting sqref="C33:D34">
+    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33:D33">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+  <conditionalFormatting sqref="C35:D35">
+    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:C17">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+  <conditionalFormatting sqref="C17:C19">
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:C9">
-    <cfRule type="duplicateValues" dxfId="2" priority="8"/>
+  <conditionalFormatting sqref="C40:D40">
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:C9">
-    <cfRule type="duplicateValues" dxfId="1" priority="9"/>
+  <conditionalFormatting sqref="C5:C12">
+    <cfRule type="duplicateValues" dxfId="4" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38:D38">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="C8:C12">
+    <cfRule type="duplicateValues" dxfId="3" priority="11"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Probability" prompt="Probability [0..1] of each item to appear._x000a_The sum of all the items should be 1." sqref="F25">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Probability" prompt="Probability [0..1] of each item to appear._x000a_The sum of all the items should be 1." sqref="F27">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D22:D25">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D24:D27">
       <formula1>"suit, pet, dragon"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E22:E25">
-      <formula1>$C$30:$C$33</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E24:E27">
+      <formula1>$C$32:$C$35</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed decimal separator from comma to dot
Former-commit-id: 689fcc15057fb01717b58adaf5f113bccb15b9c4
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gatcha.xlsx
+++ b/Docs/Content/HungryDragonContent_Gatcha.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msana/Workspace/Dragon/client_ios/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5F47BA09-6C69-084C-A7DA-AE62378B9015}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11085"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29260" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gacha" sheetId="1" r:id="rId1"/>
@@ -293,7 +294,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -601,171 +602,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1341,6 +1177,81 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1478,6 +1389,96 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1492,63 +1493,63 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="eggDefinitions" displayName="eggDefinitions" ref="B4:L12" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
-  <autoFilter ref="B4:L12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="eggDefinitions" displayName="eggDefinitions" ref="B4:L12" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+  <autoFilter ref="B4:L12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="{eggDefinitions}" dataDxfId="43"/>
-    <tableColumn id="6" name="[sku]" dataDxfId="42"/>
-    <tableColumn id="4" name="[pricePC]" dataDxfId="41"/>
-    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="40"/>
-    <tableColumn id="8" name="[weightCommon]" dataDxfId="2"/>
-    <tableColumn id="9" name="[weightRare]" dataDxfId="1"/>
-    <tableColumn id="11" name="[weightEpic]" dataDxfId="0"/>
-    <tableColumn id="10" name="[prefabPath]" dataDxfId="39"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="38"/>
-    <tableColumn id="2" name="[icon]"/>
-    <tableColumn id="3" name="[trackingSku]"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{eggDefinitions}" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[sku]" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[pricePC]" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[incubationMinutes]" dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[weightCommon]" dataDxfId="30"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[weightRare]" dataDxfId="29"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[weightEpic]" dataDxfId="28"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[prefabPath]" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[tidName]" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[icon]"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[trackingSku]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="eggRewardDefinitions" displayName="eggRewardDefinitions" ref="B23:I27" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
-  <autoFilter ref="B23:I27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="eggRewardDefinitions" displayName="eggRewardDefinitions" ref="B23:I27" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+  <autoFilter ref="B23:I27" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="33"/>
-    <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[type]" dataDxfId="32"/>
-    <tableColumn id="6" name="[rarity]" dataDxfId="31"/>
-    <tableColumn id="4" name="[droprate]" dataDxfId="30"/>
-    <tableColumn id="7" name="[duplicateFragmentsGiven]" dataDxfId="29"/>
-    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="28"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{eggRewardDefinitions}" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[type]" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[rarity]" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[droprate]" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[duplicateFragmentsGiven]" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[duplicateCoinsGiven]" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[tidName]" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="rarityDefinitions" displayName="rarityDefinitions" ref="B31:E35" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
-  <autoFilter ref="B31:E35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="rarityDefinitions" displayName="rarityDefinitions" ref="B31:E35" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="B31:E35" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="22"/>
-    <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[order]" dataDxfId="21"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{rarityDefinitions}" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="[order]" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="[tidName]" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="eggDefinitions26" displayName="eggDefinitions26" ref="B16:E19" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
-  <autoFilter ref="B16:E19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="eggDefinitions26" displayName="eggDefinitions26" ref="B16:E19" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="B16:E19" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{goldenEggDefinitions}" dataDxfId="15"/>
-    <tableColumn id="6" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="4" name="[order]" dataDxfId="13"/>
-    <tableColumn id="5" name="[fragmentsRequired]" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="{goldenEggDefinitions}" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="[order]" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="[fragmentsRequired]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1816,33 +1817,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
   <dimension ref="B1:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" customWidth="1"/>
+    <col min="8" max="8" width="25.5" customWidth="1"/>
     <col min="9" max="9" width="38" customWidth="1"/>
     <col min="10" max="10" width="45" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.28515625" customWidth="1"/>
+    <col min="11" max="11" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:25" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:25" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:25" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>66</v>
       </c>
@@ -1870,7 +1871,7 @@
       <c r="X2" s="8"/>
       <c r="Y2" s="8"/>
     </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
@@ -1878,7 +1879,7 @@
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="2:25" ht="103.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:25" ht="103" x14ac:dyDescent="0.2">
       <c r="B4" s="16" t="s">
         <v>65</v>
       </c>
@@ -1913,7 +1914,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1926,15 +1927,9 @@
       <c r="E5" s="29">
         <v>360</v>
       </c>
-      <c r="F5" s="20">
-        <v>1</v>
-      </c>
-      <c r="G5" s="20">
-        <v>2</v>
-      </c>
-      <c r="H5" s="20">
-        <v>3</v>
-      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
       <c r="I5" s="28" t="s">
         <v>59</v>
       </c>
@@ -1948,7 +1943,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B6" s="12" t="s">
         <v>1</v>
       </c>
@@ -1961,15 +1956,9 @@
       <c r="E6" s="29">
         <v>0</v>
       </c>
-      <c r="F6" s="20">
-        <v>1</v>
-      </c>
-      <c r="G6" s="20">
-        <v>2</v>
-      </c>
-      <c r="H6" s="20">
-        <v>3</v>
-      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
       <c r="I6" s="28" t="s">
         <v>49</v>
       </c>
@@ -1983,7 +1972,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
         <v>1</v>
       </c>
@@ -1996,15 +1985,9 @@
       <c r="E7" s="29">
         <v>0</v>
       </c>
-      <c r="F7" s="20">
-        <v>1</v>
-      </c>
-      <c r="G7" s="20">
-        <v>2</v>
-      </c>
-      <c r="H7" s="20">
-        <v>3</v>
-      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
       <c r="I7" s="28" t="s">
         <v>54</v>
       </c>
@@ -2018,7 +2001,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B8" s="35" t="s">
         <v>1</v>
       </c>
@@ -2031,15 +2014,9 @@
       <c r="E8" s="33">
         <v>0</v>
       </c>
-      <c r="F8" s="20">
-        <v>1</v>
-      </c>
-      <c r="G8" s="20">
-        <v>2</v>
-      </c>
-      <c r="H8" s="20">
-        <v>3</v>
-      </c>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
       <c r="I8" s="32" t="s">
         <v>49</v>
       </c>
@@ -2053,7 +2030,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B9" s="12" t="s">
         <v>1</v>
       </c>
@@ -2066,15 +2043,9 @@
       <c r="E9" s="29">
         <v>0</v>
       </c>
-      <c r="F9" s="20">
-        <v>1</v>
-      </c>
-      <c r="G9" s="20">
-        <v>2</v>
-      </c>
-      <c r="H9" s="20">
-        <v>3</v>
-      </c>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
       <c r="I9" s="28" t="s">
         <v>49</v>
       </c>
@@ -2088,7 +2059,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B10" s="12" t="s">
         <v>1</v>
       </c>
@@ -2123,7 +2094,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
         <v>1</v>
       </c>
@@ -2158,7 +2129,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B12" s="12" t="s">
         <v>1</v>
       </c>
@@ -2193,8 +2164,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:25" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:25" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:25" ht="24" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
         <v>45</v>
       </c>
@@ -2203,7 +2174,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -2211,7 +2182,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="2:25" ht="114" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:25" ht="113" x14ac:dyDescent="0.2">
       <c r="B16" s="16" t="s">
         <v>44</v>
       </c>
@@ -2225,7 +2196,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="12" t="s">
         <v>1</v>
       </c>
@@ -2239,7 +2210,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="12" t="s">
         <v>1</v>
       </c>
@@ -2253,7 +2224,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="12" t="s">
         <v>1</v>
       </c>
@@ -2267,7 +2238,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -2275,7 +2246,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" ht="24" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
         <v>39</v>
       </c>
@@ -2286,7 +2257,7 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" ht="30" x14ac:dyDescent="0.2">
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="E22" s="17"/>
@@ -2298,7 +2269,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="131.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" ht="130" x14ac:dyDescent="0.2">
       <c r="B23" s="16" t="s">
         <v>36</v>
       </c>
@@ -2324,7 +2295,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="12" t="s">
         <v>1</v>
       </c>
@@ -2350,7 +2321,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="12" t="s">
         <v>1</v>
       </c>
@@ -2376,7 +2347,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="12" t="s">
         <v>1</v>
       </c>
@@ -2402,7 +2373,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="12" t="s">
         <v>1</v>
       </c>
@@ -2428,8 +2399,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:9" ht="24" x14ac:dyDescent="0.3">
       <c r="B29" s="8" t="s">
         <v>21</v>
       </c>
@@ -2439,7 +2410,7 @@
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="18" t="s">
@@ -2449,7 +2420,7 @@
       <c r="F30" s="17"/>
       <c r="G30" s="17"/>
     </row>
-    <row r="31" spans="2:9" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" ht="91" x14ac:dyDescent="0.2">
       <c r="B31" s="16" t="s">
         <v>19</v>
       </c>
@@ -2463,7 +2434,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="12" t="s">
         <v>1</v>
       </c>
@@ -2477,7 +2448,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" s="12" t="s">
         <v>1</v>
       </c>
@@ -2491,7 +2462,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="12" t="s">
         <v>1</v>
       </c>
@@ -2505,7 +2476,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" s="12" t="s">
         <v>1</v>
       </c>
@@ -2519,8 +2490,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B37" s="8" t="s">
         <v>8</v>
       </c>
@@ -2530,7 +2501,7 @@
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
     </row>
-    <row r="39" spans="2:7" ht="131.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" ht="130" x14ac:dyDescent="0.2">
       <c r="B39" s="7" t="s">
         <v>7</v>
       </c>
@@ -2550,7 +2521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B40" s="4" t="s">
         <v>1</v>
       </c>
@@ -2572,41 +2543,41 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="11" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C27">
-    <cfRule type="duplicateValues" dxfId="10" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:D32">
-    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33:D34">
-    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:D35">
-    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:C19">
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40:D40">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C12">
-    <cfRule type="duplicateValues" dxfId="4" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C12">
-    <cfRule type="duplicateValues" dxfId="3" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="11"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Probability" prompt="Probability [0..1] of each item to appear._x000a_The sum of all the items should be 1." sqref="F27">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Probability" prompt="Probability [0..1] of each item to appear._x000a_The sum of all the items should be 1." sqref="F27" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D24:D27">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D24:D27" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"suit, pet, dragon"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E24:E27">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E24:E27" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>$C$32:$C$35</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Revert "changed decimal separator from comma to dot"
This reverts commit 60650a06b3c3b73f62e433c53c0a65154d909ee0 [formerly 689fcc15057fb01717b58adaf5f113bccb15b9c4].


Former-commit-id: b908f067f4d8e22a2f1ea3511e33e9d8f2bedc3f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gatcha.xlsx
+++ b/Docs/Content/HungryDragonContent_Gatcha.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msana/Workspace/Dragon/client_ios/Docs/Content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5F47BA09-6C69-084C-A7DA-AE62378B9015}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29260" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11085"/>
   </bookViews>
   <sheets>
     <sheet name="gacha" sheetId="1" r:id="rId1"/>
@@ -294,7 +293,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -602,6 +601,171 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1177,81 +1341,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1389,96 +1478,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1493,63 +1492,63 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="eggDefinitions" displayName="eggDefinitions" ref="B4:L12" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
-  <autoFilter ref="B4:L12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="eggDefinitions" displayName="eggDefinitions" ref="B4:L12" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+  <autoFilter ref="B4:L12"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{eggDefinitions}" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[sku]" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[pricePC]" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[incubationMinutes]" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[weightCommon]" dataDxfId="30"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[weightRare]" dataDxfId="29"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[weightEpic]" dataDxfId="28"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[prefabPath]" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[tidName]" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[icon]"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[trackingSku]"/>
+    <tableColumn id="1" name="{eggDefinitions}" dataDxfId="43"/>
+    <tableColumn id="6" name="[sku]" dataDxfId="42"/>
+    <tableColumn id="4" name="[pricePC]" dataDxfId="41"/>
+    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="40"/>
+    <tableColumn id="8" name="[weightCommon]" dataDxfId="2"/>
+    <tableColumn id="9" name="[weightRare]" dataDxfId="1"/>
+    <tableColumn id="11" name="[weightEpic]" dataDxfId="0"/>
+    <tableColumn id="10" name="[prefabPath]" dataDxfId="39"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="38"/>
+    <tableColumn id="2" name="[icon]"/>
+    <tableColumn id="3" name="[trackingSku]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="eggRewardDefinitions" displayName="eggRewardDefinitions" ref="B23:I27" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
-  <autoFilter ref="B23:I27" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="eggRewardDefinitions" displayName="eggRewardDefinitions" ref="B23:I27" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="B23:I27"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{eggRewardDefinitions}" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[type]" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[rarity]" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[droprate]" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[duplicateFragmentsGiven]" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[duplicateCoinsGiven]" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[tidName]" dataDxfId="15"/>
+    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="33"/>
+    <tableColumn id="2" name="[sku]"/>
+    <tableColumn id="3" name="[type]" dataDxfId="32"/>
+    <tableColumn id="6" name="[rarity]" dataDxfId="31"/>
+    <tableColumn id="4" name="[droprate]" dataDxfId="30"/>
+    <tableColumn id="7" name="[duplicateFragmentsGiven]" dataDxfId="29"/>
+    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="28"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="rarityDefinitions" displayName="rarityDefinitions" ref="B31:E35" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="B31:E35" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="rarityDefinitions" displayName="rarityDefinitions" ref="B31:E35" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+  <autoFilter ref="B31:E35"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{rarityDefinitions}" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="[order]" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="[tidName]" dataDxfId="8"/>
+    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="22"/>
+    <tableColumn id="2" name="[sku]"/>
+    <tableColumn id="3" name="[order]" dataDxfId="21"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="eggDefinitions26" displayName="eggDefinitions26" ref="B16:E19" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B16:E19" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="eggDefinitions26" displayName="eggDefinitions26" ref="B16:E19" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+  <autoFilter ref="B16:E19"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="{goldenEggDefinitions}" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="[order]" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="[fragmentsRequired]" dataDxfId="0"/>
+    <tableColumn id="1" name="{goldenEggDefinitions}" dataDxfId="15"/>
+    <tableColumn id="6" name="[sku]" dataDxfId="14"/>
+    <tableColumn id="4" name="[order]" dataDxfId="13"/>
+    <tableColumn id="5" name="[fragmentsRequired]" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1817,33 +1816,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
   <dimension ref="B1:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="33.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="27.6640625" customWidth="1"/>
-    <col min="8" max="8" width="25.5" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" customWidth="1"/>
     <col min="9" max="9" width="38" customWidth="1"/>
     <col min="10" max="10" width="45" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.33203125" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:25" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>66</v>
       </c>
@@ -1871,7 +1870,7 @@
       <c r="X2" s="8"/>
       <c r="Y2" s="8"/>
     </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
@@ -1879,7 +1878,7 @@
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="2:25" ht="103" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:25" ht="103.5" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
         <v>65</v>
       </c>
@@ -1914,7 +1913,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1927,9 +1926,15 @@
       <c r="E5" s="29">
         <v>360</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
+      <c r="F5" s="20">
+        <v>1</v>
+      </c>
+      <c r="G5" s="20">
+        <v>2</v>
+      </c>
+      <c r="H5" s="20">
+        <v>3</v>
+      </c>
       <c r="I5" s="28" t="s">
         <v>59</v>
       </c>
@@ -1943,7 +1948,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>1</v>
       </c>
@@ -1956,9 +1961,15 @@
       <c r="E6" s="29">
         <v>0</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
+      <c r="F6" s="20">
+        <v>1</v>
+      </c>
+      <c r="G6" s="20">
+        <v>2</v>
+      </c>
+      <c r="H6" s="20">
+        <v>3</v>
+      </c>
       <c r="I6" s="28" t="s">
         <v>49</v>
       </c>
@@ -1972,7 +1983,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>1</v>
       </c>
@@ -1985,9 +1996,15 @@
       <c r="E7" s="29">
         <v>0</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
+      <c r="F7" s="20">
+        <v>1</v>
+      </c>
+      <c r="G7" s="20">
+        <v>2</v>
+      </c>
+      <c r="H7" s="20">
+        <v>3</v>
+      </c>
       <c r="I7" s="28" t="s">
         <v>54</v>
       </c>
@@ -2001,7 +2018,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B8" s="35" t="s">
         <v>1</v>
       </c>
@@ -2014,9 +2031,15 @@
       <c r="E8" s="33">
         <v>0</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
+      <c r="F8" s="20">
+        <v>1</v>
+      </c>
+      <c r="G8" s="20">
+        <v>2</v>
+      </c>
+      <c r="H8" s="20">
+        <v>3</v>
+      </c>
       <c r="I8" s="32" t="s">
         <v>49</v>
       </c>
@@ -2030,7 +2053,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>1</v>
       </c>
@@ -2043,9 +2066,15 @@
       <c r="E9" s="29">
         <v>0</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
+      <c r="F9" s="20">
+        <v>1</v>
+      </c>
+      <c r="G9" s="20">
+        <v>2</v>
+      </c>
+      <c r="H9" s="20">
+        <v>3</v>
+      </c>
       <c r="I9" s="28" t="s">
         <v>49</v>
       </c>
@@ -2059,7 +2088,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
         <v>1</v>
       </c>
@@ -2094,7 +2123,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
         <v>1</v>
       </c>
@@ -2129,7 +2158,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
         <v>1</v>
       </c>
@@ -2164,8 +2193,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="2:25" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:25" ht="24" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B14" s="8" t="s">
         <v>45</v>
       </c>
@@ -2174,7 +2203,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -2182,7 +2211,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="2:25" ht="113" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:25" ht="114" x14ac:dyDescent="0.25">
       <c r="B16" s="16" t="s">
         <v>44</v>
       </c>
@@ -2196,7 +2225,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
         <v>1</v>
       </c>
@@ -2210,7 +2239,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>1</v>
       </c>
@@ -2224,7 +2253,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>1</v>
       </c>
@@ -2238,7 +2267,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -2246,7 +2275,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="2:9" ht="24" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B21" s="8" t="s">
         <v>39</v>
       </c>
@@ -2257,7 +2286,7 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="2:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="E22" s="17"/>
@@ -2269,7 +2298,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="130" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9" ht="131.25" x14ac:dyDescent="0.25">
       <c r="B23" s="16" t="s">
         <v>36</v>
       </c>
@@ -2295,7 +2324,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="12" t="s">
         <v>1</v>
       </c>
@@ -2321,7 +2350,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="12" t="s">
         <v>1</v>
       </c>
@@ -2347,7 +2376,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>1</v>
       </c>
@@ -2373,7 +2402,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
         <v>1</v>
       </c>
@@ -2399,8 +2428,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:9" ht="24" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B29" s="8" t="s">
         <v>21</v>
       </c>
@@ -2410,7 +2439,7 @@
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="18" t="s">
@@ -2420,7 +2449,7 @@
       <c r="F30" s="17"/>
       <c r="G30" s="17"/>
     </row>
-    <row r="31" spans="2:9" ht="91" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:9" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B31" s="16" t="s">
         <v>19</v>
       </c>
@@ -2434,7 +2463,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="12" t="s">
         <v>1</v>
       </c>
@@ -2448,7 +2477,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="12" t="s">
         <v>1</v>
       </c>
@@ -2462,7 +2491,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="12" t="s">
         <v>1</v>
       </c>
@@ -2476,7 +2505,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="12" t="s">
         <v>1</v>
       </c>
@@ -2490,8 +2519,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="2:7" ht="24" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B37" s="8" t="s">
         <v>8</v>
       </c>
@@ -2501,7 +2530,7 @@
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
     </row>
-    <row r="39" spans="2:7" ht="130" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:7" ht="131.25" x14ac:dyDescent="0.25">
       <c r="B39" s="7" t="s">
         <v>7</v>
       </c>
@@ -2521,7 +2550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
         <v>1</v>
       </c>
@@ -2543,41 +2572,41 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="47" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C27">
-    <cfRule type="duplicateValues" dxfId="46" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:D32">
-    <cfRule type="duplicateValues" dxfId="45" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33:D34">
-    <cfRule type="duplicateValues" dxfId="44" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:D35">
-    <cfRule type="duplicateValues" dxfId="43" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:C19">
-    <cfRule type="duplicateValues" dxfId="42" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40:D40">
-    <cfRule type="duplicateValues" dxfId="41" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C12">
-    <cfRule type="duplicateValues" dxfId="40" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C12">
-    <cfRule type="duplicateValues" dxfId="39" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="11"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Probability" prompt="Probability [0..1] of each item to appear._x000a_The sum of all the items should be 1." sqref="F27" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Probability" prompt="Probability [0..1] of each item to appear._x000a_The sum of all the items should be 1." sqref="F27">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D24:D27" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D24:D27">
       <formula1>"suit, pet, dragon"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E24:E27" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E24:E27">
       <formula1>$C$32:$C$35</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Content - Replace , per . when needed
Former-commit-id: d86ea0f6de9edf40dda3ae1ca7a08d073dceaee2
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gatcha.xlsx
+++ b/Docs/Content/HungryDragonContent_Gatcha.xlsx
@@ -601,171 +601,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1341,6 +1176,81 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1478,6 +1388,96 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1492,18 +1492,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="eggDefinitions" displayName="eggDefinitions" ref="B4:L12" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="eggDefinitions" displayName="eggDefinitions" ref="B4:L12" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="B4:L12"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="{eggDefinitions}" dataDxfId="43"/>
-    <tableColumn id="6" name="[sku]" dataDxfId="42"/>
-    <tableColumn id="4" name="[pricePC]" dataDxfId="41"/>
-    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="40"/>
-    <tableColumn id="8" name="[weightCommon]" dataDxfId="2"/>
-    <tableColumn id="9" name="[weightRare]" dataDxfId="1"/>
-    <tableColumn id="11" name="[weightEpic]" dataDxfId="0"/>
-    <tableColumn id="10" name="[prefabPath]" dataDxfId="39"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="38"/>
+    <tableColumn id="1" name="{eggDefinitions}" dataDxfId="34"/>
+    <tableColumn id="6" name="[sku]" dataDxfId="33"/>
+    <tableColumn id="4" name="[pricePC]" dataDxfId="32"/>
+    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="31"/>
+    <tableColumn id="8" name="[weightCommon]" dataDxfId="30"/>
+    <tableColumn id="9" name="[weightRare]" dataDxfId="29"/>
+    <tableColumn id="11" name="[weightEpic]" dataDxfId="28"/>
+    <tableColumn id="10" name="[prefabPath]" dataDxfId="27"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="26"/>
     <tableColumn id="2" name="[icon]"/>
     <tableColumn id="3" name="[trackingSku]"/>
   </tableColumns>
@@ -1512,43 +1512,43 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="eggRewardDefinitions" displayName="eggRewardDefinitions" ref="B23:I27" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="eggRewardDefinitions" displayName="eggRewardDefinitions" ref="B23:I27" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="B23:I27"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="33"/>
+    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="21"/>
     <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[type]" dataDxfId="32"/>
-    <tableColumn id="6" name="[rarity]" dataDxfId="31"/>
-    <tableColumn id="4" name="[droprate]" dataDxfId="30"/>
-    <tableColumn id="7" name="[duplicateFragmentsGiven]" dataDxfId="29"/>
-    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="28"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="27"/>
+    <tableColumn id="3" name="[type]" dataDxfId="20"/>
+    <tableColumn id="6" name="[rarity]" dataDxfId="19"/>
+    <tableColumn id="4" name="[droprate]" dataDxfId="18"/>
+    <tableColumn id="7" name="[duplicateFragmentsGiven]" dataDxfId="17"/>
+    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="16"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="rarityDefinitions" displayName="rarityDefinitions" ref="B31:E35" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="rarityDefinitions" displayName="rarityDefinitions" ref="B31:E35" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="B31:E35"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="22"/>
+    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="10"/>
     <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[order]" dataDxfId="21"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="20"/>
+    <tableColumn id="3" name="[order]" dataDxfId="9"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="eggDefinitions26" displayName="eggDefinitions26" ref="B16:E19" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="eggDefinitions26" displayName="eggDefinitions26" ref="B16:E19" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B16:E19"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{goldenEggDefinitions}" dataDxfId="15"/>
-    <tableColumn id="6" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="4" name="[order]" dataDxfId="13"/>
-    <tableColumn id="5" name="[fragmentsRequired]" dataDxfId="12"/>
+    <tableColumn id="1" name="{goldenEggDefinitions}" dataDxfId="3"/>
+    <tableColumn id="6" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="4" name="[order]" dataDxfId="1"/>
+    <tableColumn id="5" name="[fragmentsRequired]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1822,8 +1822,8 @@
   </sheetPr>
   <dimension ref="B1:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2572,33 +2572,33 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="11" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C27">
-    <cfRule type="duplicateValues" dxfId="10" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:D32">
-    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33:D34">
-    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:D35">
-    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:C19">
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40:D40">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C12">
-    <cfRule type="duplicateValues" dxfId="4" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C12">
-    <cfRule type="duplicateValues" dxfId="3" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="11"/>
   </conditionalFormatting>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Probability" prompt="Probability [0..1] of each item to appear._x000a_The sum of all the items should be 1." sqref="F27">
       <formula1>0</formula1>
       <formula2>1</formula2>

</xml_diff>

<commit_message>
Content - Normal eggs weights are left empty
Former-commit-id: 02a39711633d0638e881a9d73d8bef00ae2afbe8
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gatcha.xlsx
+++ b/Docs/Content/HungryDragonContent_Gatcha.xlsx
@@ -522,7 +522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -591,11 +591,134 @@
     <xf numFmtId="49" fontId="2" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="48">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -1107,130 +1230,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -1498,12 +1497,12 @@
     <tableColumn id="1" name="{eggDefinitions}" dataDxfId="34"/>
     <tableColumn id="6" name="[sku]" dataDxfId="33"/>
     <tableColumn id="4" name="[pricePC]" dataDxfId="32"/>
-    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="31"/>
-    <tableColumn id="8" name="[weightCommon]" dataDxfId="30"/>
-    <tableColumn id="9" name="[weightRare]" dataDxfId="29"/>
-    <tableColumn id="11" name="[weightEpic]" dataDxfId="28"/>
-    <tableColumn id="10" name="[prefabPath]" dataDxfId="27"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="26"/>
+    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="4"/>
+    <tableColumn id="8" name="[weightCommon]" dataDxfId="3"/>
+    <tableColumn id="9" name="[weightRare]" dataDxfId="2"/>
+    <tableColumn id="11" name="[weightEpic]" dataDxfId="0"/>
+    <tableColumn id="10" name="[prefabPath]" dataDxfId="1"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="31"/>
     <tableColumn id="2" name="[icon]"/>
     <tableColumn id="3" name="[trackingSku]"/>
   </tableColumns>
@@ -1512,43 +1511,43 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="eggRewardDefinitions" displayName="eggRewardDefinitions" ref="B23:I27" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="eggRewardDefinitions" displayName="eggRewardDefinitions" ref="B23:I27" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
   <autoFilter ref="B23:I27"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="21"/>
+    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="26"/>
     <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[type]" dataDxfId="20"/>
-    <tableColumn id="6" name="[rarity]" dataDxfId="19"/>
-    <tableColumn id="4" name="[droprate]" dataDxfId="18"/>
-    <tableColumn id="7" name="[duplicateFragmentsGiven]" dataDxfId="17"/>
-    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="16"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="15"/>
+    <tableColumn id="3" name="[type]" dataDxfId="25"/>
+    <tableColumn id="6" name="[rarity]" dataDxfId="24"/>
+    <tableColumn id="4" name="[droprate]" dataDxfId="23"/>
+    <tableColumn id="7" name="[duplicateFragmentsGiven]" dataDxfId="22"/>
+    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="21"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="rarityDefinitions" displayName="rarityDefinitions" ref="B31:E35" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="rarityDefinitions" displayName="rarityDefinitions" ref="B31:E35" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="B31:E35"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="10"/>
+    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="15"/>
     <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[order]" dataDxfId="9"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="8"/>
+    <tableColumn id="3" name="[order]" dataDxfId="14"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="eggDefinitions26" displayName="eggDefinitions26" ref="B16:E19" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="eggDefinitions26" displayName="eggDefinitions26" ref="B16:E19" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="B16:E19"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{goldenEggDefinitions}" dataDxfId="3"/>
-    <tableColumn id="6" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="4" name="[order]" dataDxfId="1"/>
-    <tableColumn id="5" name="[fragmentsRequired]" dataDxfId="0"/>
+    <tableColumn id="1" name="{goldenEggDefinitions}" dataDxfId="8"/>
+    <tableColumn id="6" name="[sku]" dataDxfId="7"/>
+    <tableColumn id="4" name="[order]" dataDxfId="6"/>
+    <tableColumn id="5" name="[fragmentsRequired]" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1822,8 +1821,8 @@
   </sheetPr>
   <dimension ref="B1:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1926,15 +1925,9 @@
       <c r="E5" s="29">
         <v>360</v>
       </c>
-      <c r="F5" s="20">
-        <v>1</v>
-      </c>
-      <c r="G5" s="20">
-        <v>2</v>
-      </c>
-      <c r="H5" s="20">
-        <v>3</v>
-      </c>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
       <c r="I5" s="28" t="s">
         <v>59</v>
       </c>
@@ -1961,15 +1954,9 @@
       <c r="E6" s="29">
         <v>0</v>
       </c>
-      <c r="F6" s="20">
-        <v>1</v>
-      </c>
-      <c r="G6" s="20">
-        <v>2</v>
-      </c>
-      <c r="H6" s="20">
-        <v>3</v>
-      </c>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
       <c r="I6" s="28" t="s">
         <v>49</v>
       </c>
@@ -1996,15 +1983,9 @@
       <c r="E7" s="29">
         <v>0</v>
       </c>
-      <c r="F7" s="20">
-        <v>1</v>
-      </c>
-      <c r="G7" s="20">
-        <v>2</v>
-      </c>
-      <c r="H7" s="20">
-        <v>3</v>
-      </c>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
       <c r="I7" s="28" t="s">
         <v>54</v>
       </c>
@@ -2031,15 +2012,9 @@
       <c r="E8" s="33">
         <v>0</v>
       </c>
-      <c r="F8" s="20">
-        <v>1</v>
-      </c>
-      <c r="G8" s="20">
-        <v>2</v>
-      </c>
-      <c r="H8" s="20">
-        <v>3</v>
-      </c>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
       <c r="I8" s="32" t="s">
         <v>49</v>
       </c>
@@ -2066,15 +2041,9 @@
       <c r="E9" s="29">
         <v>0</v>
       </c>
-      <c r="F9" s="20">
-        <v>1</v>
-      </c>
-      <c r="G9" s="20">
-        <v>2</v>
-      </c>
-      <c r="H9" s="20">
-        <v>3</v>
-      </c>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
       <c r="I9" s="28" t="s">
         <v>49</v>
       </c>
@@ -2101,13 +2070,13 @@
       <c r="E10" s="29">
         <v>0</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="40">
         <v>0</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="40">
         <v>2</v>
       </c>
-      <c r="H10" s="29" t="s">
+      <c r="H10" s="40" t="s">
         <v>75</v>
       </c>
       <c r="I10" s="28" t="s">
@@ -2136,13 +2105,13 @@
       <c r="E11" s="29">
         <v>0</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="40">
         <v>0</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="40">
         <v>0</v>
       </c>
-      <c r="H11" s="29">
+      <c r="H11" s="40">
         <v>1</v>
       </c>
       <c r="I11" s="28" t="s">
@@ -2171,13 +2140,13 @@
       <c r="E12" s="29">
         <v>0</v>
       </c>
-      <c r="F12" s="29">
-        <v>1</v>
-      </c>
-      <c r="G12" s="29" t="s">
+      <c r="F12" s="40">
+        <v>1</v>
+      </c>
+      <c r="G12" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="H12" s="29" t="s">
+      <c r="H12" s="40" t="s">
         <v>74</v>
       </c>
       <c r="I12" s="28" t="s">
@@ -2611,12 +2580,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="4">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Content - Fix prefab names that were wrong in content
Former-commit-id: e3c676c5fc8d887d8d96e43c3454173b2f78ff8f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gatcha.xlsx
+++ b/Docs/Content/HungryDragonContent_Gatcha.xlsx
@@ -254,12 +254,6 @@
     <t>3.8</t>
   </si>
   <si>
-    <t>PF_EggRareGuaranteed</t>
-  </si>
-  <si>
-    <t>PF_EggEpicGuaranteed</t>
-  </si>
-  <si>
     <t>PF_EggBetterRates</t>
   </si>
   <si>
@@ -288,6 +282,12 @@
   </si>
   <si>
     <t>egg_better</t>
+  </si>
+  <si>
+    <t>PF_EggRare</t>
+  </si>
+  <si>
+    <t>PF_EggEpic</t>
   </si>
 </sst>
 </file>
@@ -1821,8 +1821,8 @@
   </sheetPr>
   <dimension ref="B1:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2080,16 +2080,16 @@
         <v>75</v>
       </c>
       <c r="I10" s="28" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K10" s="26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L10" s="26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.25">
@@ -2115,16 +2115,16 @@
         <v>1</v>
       </c>
       <c r="I11" s="28" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="J11" s="27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K11" s="26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L11" s="26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
@@ -2150,16 +2150,16 @@
         <v>74</v>
       </c>
       <c r="I12" s="28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J12" s="27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K12" s="26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L12" s="26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Content - GF duplicates / Pets specials are now Epic / Initial GF value
Former-commit-id: 0a08762587b8221429e04b591088960e86cd5361
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gatcha.xlsx
+++ b/Docs/Content/HungryDragonContent_Gatcha.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="gacha" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1821,8 +1821,8 @@
   </sheetPr>
   <dimension ref="B1:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2310,7 +2310,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H24" s="19">
         <v>100</v>
@@ -2336,7 +2336,7 @@
         <v>2</v>
       </c>
       <c r="G25" s="19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H25" s="19">
         <v>300</v>
@@ -2362,7 +2362,7 @@
         <v>3</v>
       </c>
       <c r="G26" s="19">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H26" s="19">
         <v>500</v>

</xml_diff>

<commit_message>
Content - GF balancing for LAB
Former-commit-id: 6c29f06a8bfceb0a262494df66444c66c0b27123
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gatcha.xlsx
+++ b/Docs/Content/HungryDragonContent_Gatcha.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="gacha" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -559,87 +559,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="38">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1262,6 +1182,76 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1276,18 +1266,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="eggDefinitions" displayName="eggDefinitions" ref="B4:L11" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="eggDefinitions" displayName="eggDefinitions" ref="B4:L11" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
   <autoFilter ref="B4:L11"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="{eggDefinitions}" dataDxfId="34"/>
-    <tableColumn id="6" name="[sku]" dataDxfId="33"/>
-    <tableColumn id="4" name="[pricePC]" dataDxfId="32"/>
-    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="31"/>
-    <tableColumn id="8" name="[weightCommon]" dataDxfId="30"/>
-    <tableColumn id="9" name="[weightRare]" dataDxfId="29"/>
-    <tableColumn id="11" name="[weightEpic]" dataDxfId="28"/>
-    <tableColumn id="10" name="[prefabPath]" dataDxfId="27"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="26"/>
+    <tableColumn id="1" name="{eggDefinitions}" dataDxfId="26"/>
+    <tableColumn id="6" name="[sku]" dataDxfId="25"/>
+    <tableColumn id="4" name="[pricePC]" dataDxfId="24"/>
+    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="23"/>
+    <tableColumn id="8" name="[weightCommon]" dataDxfId="22"/>
+    <tableColumn id="9" name="[weightRare]" dataDxfId="21"/>
+    <tableColumn id="11" name="[weightEpic]" dataDxfId="20"/>
+    <tableColumn id="10" name="[prefabPath]" dataDxfId="19"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="18"/>
     <tableColumn id="2" name="[icon]"/>
     <tableColumn id="3" name="[trackingSku]"/>
   </tableColumns>
@@ -1296,30 +1286,30 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="eggRewardDefinitions" displayName="eggRewardDefinitions" ref="B16:I19" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="eggRewardDefinitions" displayName="eggRewardDefinitions" ref="B16:I19" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B16:I19"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="21"/>
+    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="13"/>
     <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[type]" dataDxfId="20"/>
-    <tableColumn id="6" name="[rarity]" dataDxfId="19"/>
-    <tableColumn id="4" name="[droprate]" dataDxfId="18"/>
-    <tableColumn id="7" name="[duplicateFragmentsGiven]" dataDxfId="17"/>
-    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="16"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="15"/>
+    <tableColumn id="3" name="[type]" dataDxfId="12"/>
+    <tableColumn id="6" name="[rarity]" dataDxfId="11"/>
+    <tableColumn id="4" name="[droprate]" dataDxfId="10"/>
+    <tableColumn id="7" name="[duplicateFragmentsGiven]" dataDxfId="9"/>
+    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="8"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="rarityDefinitions" displayName="rarityDefinitions" ref="B23:E26" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="rarityDefinitions" displayName="rarityDefinitions" ref="B23:E26" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="B23:E26"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="10"/>
+    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="2"/>
     <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[order]" dataDxfId="9"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="8"/>
+    <tableColumn id="3" name="[order]" dataDxfId="1"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1594,7 +1584,7 @@
   <dimension ref="B1:Y31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,7 +1969,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="19">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H17" s="19">
         <v>100</v>
@@ -2005,7 +1995,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="19">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="H18" s="19">
         <v>300</v>
@@ -2031,7 +2021,7 @@
         <v>3</v>
       </c>
       <c r="G19" s="19">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="H19" s="19">
         <v>500</v>
@@ -2170,25 +2160,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C17">
-    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:D24">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:D26">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:D31">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:C11">
-    <cfRule type="duplicateValues" dxfId="2" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C11">
-    <cfRule type="duplicateValues" dxfId="1" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C19">
-    <cfRule type="duplicateValues" dxfId="0" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="13"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D17:D19">

</xml_diff>

<commit_message>
Content - Change GF given by pet duplicates
Former-commit-id: 2a9fc26fbbf50d0f89c99b844f8d76e548f87d87
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gatcha.xlsx
+++ b/Docs/Content/HungryDragonContent_Gatcha.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="gacha" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1583,8 +1583,8 @@
   </sheetPr>
   <dimension ref="B1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1969,7 +1969,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="19">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H17" s="19">
         <v>100</v>

</xml_diff>

<commit_message>
Content - Add new dailyRewards egg to the lsit
Former-commit-id: 0f1d883c4c27dda81d01ab4537e803774fc3612b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gatcha.xlsx
+++ b/Docs/Content/HungryDragonContent_Gatcha.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="gacha" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="75">
   <si>
     <t>dynamicGatcha</t>
   </si>
@@ -246,13 +246,16 @@
   </si>
   <si>
     <t>PF_EggEpic</t>
+  </si>
+  <si>
+    <t>egg_dailyLogin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,6 +291,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -480,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -555,11 +565,82 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="38">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1182,76 +1263,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1266,18 +1277,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="eggDefinitions" displayName="eggDefinitions" ref="B4:L11" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
-  <autoFilter ref="B4:L11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="eggDefinitions" displayName="eggDefinitions" ref="B4:L12" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="B4:L12"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="{eggDefinitions}" dataDxfId="26"/>
-    <tableColumn id="6" name="[sku]" dataDxfId="25"/>
-    <tableColumn id="4" name="[pricePC]" dataDxfId="24"/>
-    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="23"/>
-    <tableColumn id="8" name="[weightCommon]" dataDxfId="22"/>
-    <tableColumn id="9" name="[weightRare]" dataDxfId="21"/>
-    <tableColumn id="11" name="[weightEpic]" dataDxfId="20"/>
-    <tableColumn id="10" name="[prefabPath]" dataDxfId="19"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="18"/>
+    <tableColumn id="1" name="{eggDefinitions}" dataDxfId="33"/>
+    <tableColumn id="6" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="4" name="[pricePC]" dataDxfId="31"/>
+    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="30"/>
+    <tableColumn id="8" name="[weightCommon]" dataDxfId="29"/>
+    <tableColumn id="9" name="[weightRare]" dataDxfId="28"/>
+    <tableColumn id="11" name="[weightEpic]" dataDxfId="27"/>
+    <tableColumn id="10" name="[prefabPath]" dataDxfId="26"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="25"/>
     <tableColumn id="2" name="[icon]"/>
     <tableColumn id="3" name="[trackingSku]"/>
   </tableColumns>
@@ -1286,30 +1297,30 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="eggRewardDefinitions" displayName="eggRewardDefinitions" ref="B16:I19" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
-  <autoFilter ref="B16:I19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="eggRewardDefinitions" displayName="eggRewardDefinitions" ref="B17:I20" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+  <autoFilter ref="B17:I20"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="13"/>
+    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="20"/>
     <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[type]" dataDxfId="12"/>
-    <tableColumn id="6" name="[rarity]" dataDxfId="11"/>
-    <tableColumn id="4" name="[droprate]" dataDxfId="10"/>
-    <tableColumn id="7" name="[duplicateFragmentsGiven]" dataDxfId="9"/>
-    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="8"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="7"/>
+    <tableColumn id="3" name="[type]" dataDxfId="19"/>
+    <tableColumn id="6" name="[rarity]" dataDxfId="18"/>
+    <tableColumn id="4" name="[droprate]" dataDxfId="17"/>
+    <tableColumn id="7" name="[duplicateFragmentsGiven]" dataDxfId="16"/>
+    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="15"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="rarityDefinitions" displayName="rarityDefinitions" ref="B23:E26" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="B23:E26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="rarityDefinitions" displayName="rarityDefinitions" ref="B24:E27" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="B24:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="2"/>
+    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="9"/>
     <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[order]" dataDxfId="1"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="0"/>
+    <tableColumn id="3" name="[order]" dataDxfId="8"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1581,10 +1592,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="B1:Y31"/>
+  <dimension ref="B1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1600,6 +1611,7 @@
     <col min="9" max="9" width="38" customWidth="1"/>
     <col min="10" max="10" width="45" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1895,87 +1907,90 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-    </row>
-    <row r="14" spans="2:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B14" s="8" t="s">
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B12" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="20">
+        <v>0</v>
+      </c>
+      <c r="E12" s="29">
+        <v>0</v>
+      </c>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="L12" s="26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="2:25" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B15" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="2:25" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17" t="s">
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="2:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H16" s="18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="2:25" ht="131.25" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
+    <row r="17" spans="2:9" ht="131.25" x14ac:dyDescent="0.25">
+      <c r="B17" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C17" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D17" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E17" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F17" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="G17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H17" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I17" s="13" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="20">
-        <v>1</v>
-      </c>
-      <c r="G17" s="19">
-        <v>10</v>
-      </c>
-      <c r="H17" s="19">
-        <v>100</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -1983,25 +1998,25 @@
         <v>1</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D18" s="21" t="s">
         <v>20</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F18" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18" s="19">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="H18" s="19">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -2009,74 +2024,86 @@
         <v>1</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D19" s="21" t="s">
         <v>20</v>
       </c>
       <c r="E19" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="20">
+        <v>2</v>
+      </c>
+      <c r="G19" s="19">
+        <v>50</v>
+      </c>
+      <c r="H19" s="19">
+        <v>300</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="20">
+      <c r="F20" s="20">
         <v>3</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G20" s="19">
         <v>100</v>
       </c>
-      <c r="H19" s="19">
+      <c r="H20" s="19">
         <v>500</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I20" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B21" s="8" t="s">
+    <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18" t="s">
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-    </row>
-    <row r="23" spans="2:9" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="16" t="s">
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+    </row>
+    <row r="24" spans="2:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="B24" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C24" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D24" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E24" s="13" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="10">
-        <v>0</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
@@ -2084,13 +2111,13 @@
         <v>1</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D25" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
@@ -2098,94 +2125,108 @@
         <v>1</v>
       </c>
       <c r="C26" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="10">
+        <v>1</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D27" s="10">
         <v>2</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E27" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B28" s="8" t="s">
+    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B29" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-    </row>
-    <row r="30" spans="2:9" ht="131.25" x14ac:dyDescent="0.25">
-      <c r="B30" s="7" t="s">
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="31" spans="2:9" ht="131.25" x14ac:dyDescent="0.25">
+      <c r="B31" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C31" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D31" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E31" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F31" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="G31" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D32" s="2">
         <v>1</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E32" s="1">
         <v>4</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F32" s="1">
         <v>0.01</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G32" s="1">
         <v>1.4</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C17">
-    <cfRule type="duplicateValues" dxfId="37" priority="6"/>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:D24">
-    <cfRule type="duplicateValues" dxfId="36" priority="4"/>
+  <conditionalFormatting sqref="C25:D25">
+    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25:D26">
-    <cfRule type="duplicateValues" dxfId="35" priority="5"/>
+  <conditionalFormatting sqref="C26:D27">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31:D31">
-    <cfRule type="duplicateValues" dxfId="34" priority="1"/>
+  <conditionalFormatting sqref="C32:D32">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:C11">
-    <cfRule type="duplicateValues" dxfId="33" priority="11"/>
+  <conditionalFormatting sqref="C7:C12">
+    <cfRule type="duplicateValues" dxfId="2" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:C11">
-    <cfRule type="duplicateValues" dxfId="32" priority="12"/>
+  <conditionalFormatting sqref="C5:C12">
+    <cfRule type="duplicateValues" dxfId="1" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18:C19">
-    <cfRule type="duplicateValues" dxfId="31" priority="13"/>
+  <conditionalFormatting sqref="C19:C20">
+    <cfRule type="duplicateValues" dxfId="0" priority="13"/>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D17:D19">
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D18:D20">
       <formula1>"suit, pet, dragon"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E17:E19">
-      <formula1>$C$24:$C$26</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E18:E20">
+      <formula1>$C$25:$C$27</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Duplicated pets now reward coins or gems
Former-commit-id: 75c67179199dc179cb1141f57e710e9ea9ec00f9
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gatcha.xlsx
+++ b/Docs/Content/HungryDragonContent_Gatcha.xlsx
@@ -110,9 +110,6 @@
     <t>[duplicateCoinsGiven]</t>
   </si>
   <si>
-    <t>[duplicateFragmentsGiven]</t>
-  </si>
-  <si>
     <t>[droprate]</t>
   </si>
   <si>
@@ -249,6 +246,9 @@
   </si>
   <si>
     <t>egg_dailyLogin</t>
+  </si>
+  <si>
+    <t>[duplicateGemsGiven]</t>
   </si>
 </sst>
 </file>
@@ -1305,7 +1305,7 @@
     <tableColumn id="3" name="[type]" dataDxfId="12"/>
     <tableColumn id="6" name="[rarity]" dataDxfId="11"/>
     <tableColumn id="4" name="[droprate]" dataDxfId="10"/>
-    <tableColumn id="7" name="[duplicateFragmentsGiven]" dataDxfId="9"/>
+    <tableColumn id="7" name="[duplicateGemsGiven]" dataDxfId="9"/>
     <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="8"/>
     <tableColumn id="5" name="[tidName]" dataDxfId="7"/>
   </tableColumns>
@@ -1595,7 +1595,7 @@
   <dimension ref="B1:Y32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1617,7 +1617,7 @@
     <row r="1" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -1653,37 +1653,37 @@
     </row>
     <row r="4" spans="2:25" ht="103.5" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F4" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="H4" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="H4" s="39" t="s">
-        <v>58</v>
-      </c>
       <c r="I4" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J4" s="37" t="s">
         <v>15</v>
       </c>
       <c r="K4" s="37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L4" s="37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
@@ -1691,7 +1691,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="20">
         <v>0</v>
@@ -1703,16 +1703,16 @@
       <c r="G5" s="41"/>
       <c r="H5" s="41"/>
       <c r="I5" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J5" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
@@ -1720,7 +1720,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="20">
         <v>10</v>
@@ -1732,16 +1732,16 @@
       <c r="G6" s="41"/>
       <c r="H6" s="41"/>
       <c r="I6" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J6" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
@@ -1749,7 +1749,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="34">
         <v>0</v>
@@ -1761,16 +1761,16 @@
       <c r="G7" s="41"/>
       <c r="H7" s="41"/>
       <c r="I7" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J7" s="31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K7" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L7" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.25">
@@ -1778,7 +1778,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="20">
         <v>0</v>
@@ -1790,16 +1790,16 @@
       <c r="G8" s="41"/>
       <c r="H8" s="41"/>
       <c r="I8" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" s="26" t="s">
         <v>39</v>
-      </c>
-      <c r="J8" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="K8" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="L8" s="26" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.25">
@@ -1807,7 +1807,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" s="20">
         <v>0</v>
@@ -1822,19 +1822,19 @@
         <v>2</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I9" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J9" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L9" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.25">
@@ -1842,7 +1842,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" s="20">
         <v>0</v>
@@ -1860,16 +1860,16 @@
         <v>1</v>
       </c>
       <c r="I10" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K10" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L10" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.25">
@@ -1877,7 +1877,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="20">
         <v>0</v>
@@ -1889,22 +1889,22 @@
         <v>1</v>
       </c>
       <c r="G11" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="40" t="s">
-        <v>60</v>
-      </c>
       <c r="I11" s="28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J11" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K11" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L11" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
@@ -1912,7 +1912,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" s="20">
         <v>0</v>
@@ -1924,16 +1924,16 @@
       <c r="G12" s="40"/>
       <c r="H12" s="40"/>
       <c r="I12" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J12" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K12" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L12" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1946,7 +1946,7 @@
     </row>
     <row r="15" spans="2:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B15" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1961,30 +1961,30 @@
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" ht="131.25" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="118.5" x14ac:dyDescent="0.25">
       <c r="B17" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="H17" s="22" t="s">
         <v>27</v>
@@ -2009,11 +2009,9 @@
       <c r="F18" s="20">
         <v>1</v>
       </c>
-      <c r="G18" s="19">
-        <v>10</v>
-      </c>
+      <c r="G18" s="19"/>
       <c r="H18" s="19">
-        <v>100</v>
+        <v>5000</v>
       </c>
       <c r="I18" s="9" t="s">
         <v>25</v>
@@ -2035,11 +2033,9 @@
       <c r="F19" s="20">
         <v>2</v>
       </c>
-      <c r="G19" s="19">
-        <v>50</v>
-      </c>
+      <c r="G19" s="19"/>
       <c r="H19" s="19">
-        <v>300</v>
+        <v>10000</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>23</v>
@@ -2062,11 +2058,9 @@
         <v>3</v>
       </c>
       <c r="G20" s="19">
-        <v>100</v>
-      </c>
-      <c r="H20" s="19">
-        <v>500</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="H20" s="19"/>
       <c r="I20" s="9" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Egg Definitions: Content - Added tidDesc column.
Former-commit-id: a1973e836c548f267359bce647ce39ef0e3215cf
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gatcha.xlsx
+++ b/Docs/Content/HungryDragonContent_Gatcha.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client_iOS/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C2C5E4-1820-6D4E-AD6A-3594262E4BA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11085"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gacha" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="81">
   <si>
     <t>dynamicGatcha</t>
   </si>
@@ -249,12 +250,30 @@
   </si>
   <si>
     <t>[duplicateGemsGiven]</t>
+  </si>
+  <si>
+    <t>[tidDesc]</t>
+  </si>
+  <si>
+    <t>TID_EGG_STANDARD_DESC</t>
+  </si>
+  <si>
+    <t>TID_EGG_PREMIUM_DESC</t>
+  </si>
+  <si>
+    <t>TID_EGG_RARE_DESC</t>
+  </si>
+  <si>
+    <t>TID_EGG_EPIC_DESC</t>
+  </si>
+  <si>
+    <t>TID_EGG_BETTER_DESC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -490,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -539,7 +558,6 @@
       <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -570,7 +588,152 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="41">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -661,13 +824,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -677,6 +833,13 @@
         <top style="thin">
           <color auto="1"/>
         </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -879,13 +1042,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -895,6 +1051,13 @@
         <top style="thin">
           <color auto="1"/>
         </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -1159,13 +1322,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -1175,6 +1331,13 @@
         <top style="thin">
           <color auto="1"/>
         </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -1192,146 +1355,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1347,50 +1370,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="eggDefinitions5" displayName="eggDefinitions5" ref="B4:L12" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="28" tableBorderDxfId="29" totalsRowBorderDxfId="27">
-  <autoFilter ref="B4:L12"/>
-  <tableColumns count="11">
-    <tableColumn id="1" name="{eggDefinitions}" dataDxfId="26"/>
-    <tableColumn id="6" name="[sku]" dataDxfId="25"/>
-    <tableColumn id="4" name="[pricePC]" dataDxfId="24"/>
-    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="23"/>
-    <tableColumn id="8" name="[weightCommon]" dataDxfId="22"/>
-    <tableColumn id="9" name="[weightRare]" dataDxfId="21"/>
-    <tableColumn id="11" name="[weightEpic]" dataDxfId="20"/>
-    <tableColumn id="10" name="[prefabPath]" dataDxfId="19"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="18"/>
-    <tableColumn id="2" name="[icon]"/>
-    <tableColumn id="3" name="[trackingSku]"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="eggDefinitions5" displayName="eggDefinitions5" ref="B4:M12" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
+  <autoFilter ref="B4:M12" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{eggDefinitions}" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[sku]" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[pricePC]" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[incubationMinutes]" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[weightCommon]" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[weightRare]" dataDxfId="31"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[weightEpic]" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[prefabPath]" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[tidName]" dataDxfId="28"/>
+    <tableColumn id="12" xr3:uid="{5F0CEE5C-AAE0-9649-BD4A-A3E925A355B5}" name="[tidDesc]" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[icon]" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[trackingSku]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="eggRewardDefinitions6" displayName="eggRewardDefinitions6" ref="B17:I20" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
-  <autoFilter ref="B17:I20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="eggRewardDefinitions6" displayName="eggRewardDefinitions6" ref="B17:I20" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+  <autoFilter ref="B17:I20" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[type]" dataDxfId="12"/>
-    <tableColumn id="6" name="[rarity]" dataDxfId="11"/>
-    <tableColumn id="4" name="[droprate]" dataDxfId="10"/>
-    <tableColumn id="7" name="[duplicateGemsGiven]" dataDxfId="9"/>
-    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="8"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{eggRewardDefinitions}" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[type]" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[rarity]" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[droprate]" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[duplicateGemsGiven]" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[duplicateCoinsGiven]" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[tidName]" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="rarityDefinitions7" displayName="rarityDefinitions7" ref="B24:E27" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
-  <autoFilter ref="B24:E27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="rarityDefinitions7" displayName="rarityDefinitions7" ref="B24:E27" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="B24:E27" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="2"/>
-    <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[order]" dataDxfId="1"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{rarityDefinitions}" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="[order]" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="[tidName]" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1658,34 +1682,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
   <dimension ref="B1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" customWidth="1"/>
+    <col min="8" max="8" width="25.5" customWidth="1"/>
     <col min="9" max="9" width="38" customWidth="1"/>
     <col min="10" max="10" width="45" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.28515625" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:25" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:25" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:25" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>51</v>
       </c>
@@ -1713,7 +1737,7 @@
       <c r="X2" s="8"/>
       <c r="Y2" s="8"/>
     </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
@@ -1721,7 +1745,7 @@
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="2:25" ht="103.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:25" ht="103" x14ac:dyDescent="0.2">
       <c r="B4" s="16" t="s">
         <v>50</v>
       </c>
@@ -1731,32 +1755,35 @@
       <c r="D4" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="39" t="s">
+      <c r="H4" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="J4" s="37" t="s">
+      <c r="J4" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="K4" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="L4" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="L4" s="37" t="s">
+      <c r="M4" s="36" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1766,247 +1793,271 @@
       <c r="D5" s="20">
         <v>0</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="28">
         <v>360</v>
       </c>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="28" t="s">
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="J5" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="L5" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" s="35" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="29" t="s">
         <v>40</v>
       </c>
       <c r="D6" s="20">
         <v>10</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="28">
         <v>0</v>
       </c>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="28" t="s">
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="J6" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="L6" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" s="35" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B7" s="35" t="s">
+    <row r="7" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B7" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="33">
         <v>0</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="32">
         <v>0</v>
       </c>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="32" t="s">
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="31" t="s">
+      <c r="J7" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="K7" s="26" t="s">
+      <c r="K7" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="L7" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="L7" s="26" t="s">
+      <c r="M7" s="30" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="29" t="s">
         <v>39</v>
       </c>
       <c r="D8" s="20">
         <v>0</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="28">
         <v>0</v>
       </c>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="28" t="s">
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="27" t="s">
+      <c r="J8" s="26" t="s">
         <v>37</v>
       </c>
       <c r="K8" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="L8" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="26" t="s">
+      <c r="M8" s="26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B9" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="29" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="20">
         <v>0</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="28">
         <v>0</v>
       </c>
-      <c r="F9" s="40">
+      <c r="F9" s="39">
         <v>0</v>
       </c>
-      <c r="G9" s="40">
+      <c r="G9" s="39">
         <v>2</v>
       </c>
-      <c r="H9" s="40" t="s">
+      <c r="H9" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="28" t="s">
+      <c r="I9" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="26" t="s">
         <v>62</v>
       </c>
       <c r="K9" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="L9" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="L9" s="26" t="s">
+      <c r="M9" s="26" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B10" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="29" t="s">
         <v>53</v>
       </c>
       <c r="D10" s="20">
         <v>0</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="28">
         <v>0</v>
       </c>
-      <c r="F10" s="40">
+      <c r="F10" s="39">
         <v>0</v>
       </c>
-      <c r="G10" s="40">
+      <c r="G10" s="39">
         <v>0</v>
       </c>
-      <c r="H10" s="40">
+      <c r="H10" s="39">
         <v>1</v>
       </c>
-      <c r="I10" s="28" t="s">
+      <c r="I10" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="J10" s="27" t="s">
+      <c r="J10" s="26" t="s">
         <v>63</v>
       </c>
       <c r="K10" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="L10" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="L10" s="26" t="s">
+      <c r="M10" s="26" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="29" t="s">
         <v>54</v>
       </c>
       <c r="D11" s="20">
         <v>0</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="28">
         <v>0</v>
       </c>
-      <c r="F11" s="40">
+      <c r="F11" s="39">
         <v>1</v>
       </c>
-      <c r="G11" s="40" t="s">
+      <c r="G11" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="40" t="s">
+      <c r="H11" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="28" t="s">
+      <c r="I11" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="J11" s="27" t="s">
+      <c r="J11" s="26" t="s">
         <v>64</v>
       </c>
       <c r="K11" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="L11" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="L11" s="26" t="s">
+      <c r="M11" s="26" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B12" s="42" t="s">
+    <row r="12" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B12" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="29" t="s">
         <v>73</v>
       </c>
       <c r="D12" s="20">
         <v>0</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E12" s="28">
         <v>0</v>
       </c>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="28" t="s">
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="J12" s="27" t="s">
+      <c r="J12" s="26" t="s">
         <v>37</v>
       </c>
       <c r="K12" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="L12" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="L12" s="26" t="s">
+      <c r="M12" s="26" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -2014,7 +2065,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="2:25" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:25" ht="24" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
         <v>34</v>
       </c>
@@ -2025,7 +2076,7 @@
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="2:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:25" ht="32" x14ac:dyDescent="0.2">
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="E16" s="17"/>
@@ -2037,7 +2088,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="118.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" ht="115" x14ac:dyDescent="0.2">
       <c r="B17" s="16" t="s">
         <v>31</v>
       </c>
@@ -2063,7 +2114,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="12" t="s">
         <v>1</v>
       </c>
@@ -2087,7 +2138,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="12" t="s">
         <v>1</v>
       </c>
@@ -2111,7 +2162,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="12" t="s">
         <v>1</v>
       </c>
@@ -2135,8 +2186,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:9" ht="24" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
         <v>19</v>
       </c>
@@ -2146,7 +2197,7 @@
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="18" t="s">
@@ -2156,7 +2207,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="2:9" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" ht="91" x14ac:dyDescent="0.2">
       <c r="B24" s="16" t="s">
         <v>17</v>
       </c>
@@ -2170,7 +2221,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="12" t="s">
         <v>1</v>
       </c>
@@ -2184,7 +2235,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="12" t="s">
         <v>1</v>
       </c>
@@ -2198,7 +2249,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="12" t="s">
         <v>1</v>
       </c>
@@ -2212,8 +2263,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:9" ht="24" x14ac:dyDescent="0.3">
       <c r="B29" s="8" t="s">
         <v>8</v>
       </c>
@@ -2223,7 +2274,7 @@
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="31" spans="2:9" ht="131.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" ht="130" x14ac:dyDescent="0.2">
       <c r="B31" s="7" t="s">
         <v>7</v>
       </c>
@@ -2243,7 +2294,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="s">
         <v>1</v>
       </c>
@@ -2265,31 +2316,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C18">
-    <cfRule type="duplicateValues" dxfId="37" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:D25">
-    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:D27">
-    <cfRule type="duplicateValues" dxfId="35" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:D32">
-    <cfRule type="duplicateValues" dxfId="34" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:C12">
-    <cfRule type="duplicateValues" dxfId="33" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C12">
-    <cfRule type="duplicateValues" dxfId="32" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:C20">
-    <cfRule type="duplicateValues" dxfId="31" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D18:D20">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D18:D20" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"suit, pet, dragon"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E18:E20">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E18:E20" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$C$25:$C$27</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Rarity Definitions: Content - Changed tidName to the new ones.
Former-commit-id: 6d0f6c30999f134db8ee081363cb637d709f4e6c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gatcha.xlsx
+++ b/Docs/Content/HungryDragonContent_Gatcha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client_iOS/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C2C5E4-1820-6D4E-AD6A-3594262E4BA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F91AD0-E98E-B542-AD42-189A4959121C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,21 +54,12 @@
     <t>DYNAMIC GATCHA DEFINITIONS</t>
   </si>
   <si>
-    <t>TID_SKIN_RARITY_EPIC_NAME</t>
-  </si>
-  <si>
     <t>epic</t>
   </si>
   <si>
-    <t>TID_SKIN_RARITY_RARE_NAME</t>
-  </si>
-  <si>
     <t>rare</t>
   </si>
   <si>
-    <t>TID_SKIN_RARITY_COMMON_NAME</t>
-  </si>
-  <si>
     <t>common</t>
   </si>
   <si>
@@ -268,6 +259,15 @@
   </si>
   <si>
     <t>TID_EGG_BETTER_DESC</t>
+  </si>
+  <si>
+    <t>TID_RARITY_COMMON</t>
+  </si>
+  <si>
+    <t>TID_RARITY_RARE</t>
+  </si>
+  <si>
+    <t>TID_RARITY_EPIC</t>
   </si>
 </sst>
 </file>
@@ -590,151 +590,6 @@
   </cellStyles>
   <dxfs count="41">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1075,6 +930,81 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1356,6 +1286,76 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1370,51 +1370,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="eggDefinitions5" displayName="eggDefinitions5" ref="B4:M12" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="eggDefinitions5" displayName="eggDefinitions5" ref="B4:M12" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <autoFilter ref="B4:M12" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{eggDefinitions}" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[sku]" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[pricePC]" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[incubationMinutes]" dataDxfId="33"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[weightCommon]" dataDxfId="32"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[weightRare]" dataDxfId="31"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[weightEpic]" dataDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[prefabPath]" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[tidName]" dataDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{5F0CEE5C-AAE0-9649-BD4A-A3E925A355B5}" name="[tidDesc]" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[icon]" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[trackingSku]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{eggDefinitions}" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[sku]" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[pricePC]" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[incubationMinutes]" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[weightCommon]" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[weightRare]" dataDxfId="24"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[weightEpic]" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[prefabPath]" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[tidName]" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{5F0CEE5C-AAE0-9649-BD4A-A3E925A355B5}" name="[tidDesc]" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[icon]" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[trackingSku]" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="eggRewardDefinitions6" displayName="eggRewardDefinitions6" ref="B17:I20" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="eggRewardDefinitions6" displayName="eggRewardDefinitions6" ref="B17:I20" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B17:I20" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{eggRewardDefinitions}" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{eggRewardDefinitions}" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[type]" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[rarity]" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[droprate]" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[duplicateGemsGiven]" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[duplicateCoinsGiven]" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[tidName]" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[type]" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[rarity]" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[droprate]" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[duplicateGemsGiven]" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[duplicateCoinsGiven]" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[tidName]" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="rarityDefinitions7" displayName="rarityDefinitions7" ref="B24:E27" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="rarityDefinitions7" displayName="rarityDefinitions7" ref="B24:E27" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="B24:E27" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{rarityDefinitions}" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{rarityDefinitions}" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="[order]" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="[tidName]" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="[order]" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="[tidName]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1688,8 +1688,8 @@
   </sheetPr>
   <dimension ref="B1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1711,7 +1711,7 @@
     <row r="1" spans="2:25" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:25" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -1747,40 +1747,40 @@
     </row>
     <row r="4" spans="2:25" ht="103" x14ac:dyDescent="0.2">
       <c r="B4" s="16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G4" s="38" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H4" s="38" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I4" s="37" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J4" s="36" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K4" s="36" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L4" s="36" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="M4" s="36" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.2">
@@ -1788,7 +1788,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D5" s="20">
         <v>0</v>
@@ -1800,19 +1800,19 @@
       <c r="G5" s="40"/>
       <c r="H5" s="40"/>
       <c r="I5" s="27" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J5" s="35" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="K5" s="35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L5" s="35" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="M5" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.2">
@@ -1820,7 +1820,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D6" s="20">
         <v>10</v>
@@ -1832,19 +1832,19 @@
       <c r="G6" s="40"/>
       <c r="H6" s="40"/>
       <c r="I6" s="27" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J6" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="L6" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="35" t="s">
         <v>37</v>
-      </c>
-      <c r="K6" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="L6" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" s="35" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.2">
@@ -1852,7 +1852,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D7" s="33">
         <v>0</v>
@@ -1864,19 +1864,19 @@
       <c r="G7" s="40"/>
       <c r="H7" s="40"/>
       <c r="I7" s="31" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J7" s="30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K7" s="30" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L7" s="30" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M7" s="30" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.2">
@@ -1884,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D8" s="20">
         <v>0</v>
@@ -1896,19 +1896,19 @@
       <c r="G8" s="40"/>
       <c r="H8" s="40"/>
       <c r="I8" s="27" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J8" s="26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K8" s="26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L8" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="M8" s="26" t="s">
         <v>36</v>
-      </c>
-      <c r="M8" s="26" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.2">
@@ -1916,7 +1916,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D9" s="20">
         <v>0</v>
@@ -1931,22 +1931,22 @@
         <v>2</v>
       </c>
       <c r="H9" s="39" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J9" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="L9" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="K9" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="L9" s="26" t="s">
+      <c r="M9" s="26" t="s">
         <v>65</v>
-      </c>
-      <c r="M9" s="26" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.2">
@@ -1954,7 +1954,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D10" s="20">
         <v>0</v>
@@ -1972,19 +1972,19 @@
         <v>1</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J10" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="L10" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="K10" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="L10" s="26" t="s">
+      <c r="M10" s="26" t="s">
         <v>66</v>
-      </c>
-      <c r="M10" s="26" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.2">
@@ -1992,7 +1992,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D11" s="20">
         <v>0</v>
@@ -2004,25 +2004,25 @@
         <v>1</v>
       </c>
       <c r="G11" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" s="27" t="s">
+      <c r="J11" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="K11" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="L11" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="K11" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="L11" s="26" t="s">
+      <c r="M11" s="26" t="s">
         <v>67</v>
-      </c>
-      <c r="M11" s="26" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.2">
@@ -2030,7 +2030,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D12" s="20">
         <v>0</v>
@@ -2042,19 +2042,19 @@
       <c r="G12" s="39"/>
       <c r="H12" s="39"/>
       <c r="I12" s="27" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K12" s="26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L12" s="26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M12" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="2:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2067,7 +2067,7 @@
     </row>
     <row r="15" spans="2:25" ht="24" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -2082,36 +2082,36 @@
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="115" x14ac:dyDescent="0.2">
       <c r="B17" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
@@ -2119,13 +2119,13 @@
         <v>1</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F18" s="20">
         <v>1</v>
@@ -2135,7 +2135,7 @@
         <v>5000</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
@@ -2143,13 +2143,13 @@
         <v>1</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F19" s="20">
         <v>2</v>
@@ -2159,7 +2159,7 @@
         <v>10000</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
@@ -2167,13 +2167,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" s="20">
         <v>3</v>
@@ -2183,13 +2183,13 @@
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:9" ht="24" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -2201,7 +2201,7 @@
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
@@ -2209,16 +2209,16 @@
     </row>
     <row r="24" spans="2:9" ht="91" x14ac:dyDescent="0.2">
       <c r="B24" s="16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
@@ -2226,13 +2226,13 @@
         <v>1</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D25" s="10">
         <v>0</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
@@ -2240,13 +2240,13 @@
         <v>1</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D26" s="10">
         <v>1</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.2">
@@ -2254,13 +2254,13 @@
         <v>1</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D27" s="10">
         <v>2</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -2316,25 +2316,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C18">
-    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:D25">
-    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:D27">
-    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:D32">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:C12">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C12">
-    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:C20">
-    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="7"/>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D18:D20" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>

<commit_message>
Adding a formula to calculate final eggs probs from coef values in content
Former-commit-id: 2d076092399bb322a10fee995a260c90e8f42c50
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gatcha.xlsx
+++ b/Docs/Content/HungryDragonContent_Gatcha.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client_iOS/Docs/Content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F91AD0-E98E-B542-AD42-189A4959121C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="21360" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="gacha" sheetId="1" r:id="rId1"/>
+    <sheet name="Calculate Eggs Prob" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="87">
   <si>
     <t>dynamicGatcha</t>
   </si>
@@ -268,13 +268,31 @@
   </si>
   <si>
     <t>TID_RARITY_EPIC</t>
+  </si>
+  <si>
+    <t>COEFICIENTS</t>
+  </si>
+  <si>
+    <t>CoefG</t>
+  </si>
+  <si>
+    <t>CoefX</t>
+  </si>
+  <si>
+    <t>CoefY</t>
+  </si>
+  <si>
+    <t>DEFAULT PROB</t>
+  </si>
+  <si>
+    <t>DEFAULT PROB NORM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,6 +335,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -388,7 +413,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -505,11 +530,97 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -584,12 +695,248 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="41">
-    <dxf>
+  <dxfs count="68">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -600,7 +947,9 @@
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -612,17 +961,41 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -634,29 +1007,38 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
         <right style="thin">
           <color auto="1"/>
         </right>
@@ -671,60 +1053,41 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -736,17 +1099,264 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -764,29 +1374,7 @@
           <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -796,380 +1384,7 @@
         <top style="thin">
           <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1224,6 +1439,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1238,16 +1454,89 @@
         <top style="thin">
           <color auto="1"/>
         </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color auto="1"/>
         </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1261,13 +1550,6 @@
         <top style="thin">
           <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -1287,74 +1569,346 @@
       </font>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1370,51 +1924,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="eggDefinitions5" displayName="eggDefinitions5" ref="B4:M12" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
-  <autoFilter ref="B4:M12" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="eggDefinitions5" displayName="eggDefinitions5" ref="B4:M12" totalsRowShown="0" headerRowDxfId="49" headerRowBorderDxfId="47" tableBorderDxfId="48" totalsRowBorderDxfId="46">
+  <autoFilter ref="B4:M12"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{eggDefinitions}" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[sku]" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[pricePC]" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[incubationMinutes]" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[weightCommon]" dataDxfId="25"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[weightRare]" dataDxfId="24"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[weightEpic]" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[prefabPath]" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[tidName]" dataDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{5F0CEE5C-AAE0-9649-BD4A-A3E925A355B5}" name="[tidDesc]" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[icon]" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[trackingSku]" dataDxfId="18"/>
+    <tableColumn id="1" name="{eggDefinitions}" dataDxfId="44" totalsRowDxfId="45"/>
+    <tableColumn id="6" name="[sku]" dataDxfId="42" totalsRowDxfId="43"/>
+    <tableColumn id="4" name="[pricePC]" dataDxfId="40" totalsRowDxfId="41"/>
+    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="38" totalsRowDxfId="39"/>
+    <tableColumn id="8" name="[weightCommon]" dataDxfId="36" totalsRowDxfId="37"/>
+    <tableColumn id="9" name="[weightRare]" dataDxfId="34" totalsRowDxfId="35"/>
+    <tableColumn id="11" name="[weightEpic]" dataDxfId="32" totalsRowDxfId="33"/>
+    <tableColumn id="10" name="[prefabPath]" dataDxfId="30" totalsRowDxfId="31"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="28" totalsRowDxfId="29"/>
+    <tableColumn id="12" name="[tidDesc]" dataDxfId="26" totalsRowDxfId="27"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="24" totalsRowDxfId="25"/>
+    <tableColumn id="3" name="[trackingSku]" dataDxfId="22" totalsRowDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="eggRewardDefinitions6" displayName="eggRewardDefinitions6" ref="B17:I20" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
-  <autoFilter ref="B17:I20" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="eggRewardDefinitions6" displayName="eggRewardDefinitions6" ref="B17:I20" totalsRowShown="0" headerRowDxfId="67" headerRowBorderDxfId="66" tableBorderDxfId="65" totalsRowBorderDxfId="64">
+  <autoFilter ref="B17:I20"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{eggRewardDefinitions}" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[type]" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[rarity]" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[droprate]" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[duplicateGemsGiven]" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[duplicateCoinsGiven]" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[tidName]" dataDxfId="7"/>
+    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="63"/>
+    <tableColumn id="2" name="[sku]"/>
+    <tableColumn id="3" name="[type]" dataDxfId="62"/>
+    <tableColumn id="6" name="[rarity]" dataDxfId="61"/>
+    <tableColumn id="4" name="[droprate]" dataDxfId="60"/>
+    <tableColumn id="7" name="[duplicateGemsGiven]" dataDxfId="59"/>
+    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="58"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="rarityDefinitions7" displayName="rarityDefinitions7" ref="B24:E27" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="B24:E27" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="rarityDefinitions7" displayName="rarityDefinitions7" ref="B24:E27" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54" totalsRowBorderDxfId="53">
+  <autoFilter ref="B24:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{rarityDefinitions}" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="[order]" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="[tidName]" dataDxfId="0"/>
+    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="52"/>
+    <tableColumn id="2" name="[sku]"/>
+    <tableColumn id="3" name="[order]" dataDxfId="51"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1682,34 +2236,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
   <dimension ref="B1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="33.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="27.6640625" customWidth="1"/>
-    <col min="8" max="8" width="25.5" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" customWidth="1"/>
     <col min="9" max="9" width="38" customWidth="1"/>
     <col min="10" max="10" width="45" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.33203125" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:25" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>48</v>
       </c>
@@ -1737,7 +2291,7 @@
       <c r="X2" s="8"/>
       <c r="Y2" s="8"/>
     </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
@@ -1745,7 +2299,7 @@
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="2:25" ht="103" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:25" ht="103.5" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
         <v>47</v>
       </c>
@@ -1783,7 +2337,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1815,7 +2369,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>1</v>
       </c>
@@ -1847,7 +2401,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="34" t="s">
         <v>1</v>
       </c>
@@ -1879,7 +2433,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
         <v>1</v>
       </c>
@@ -1911,7 +2465,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>1</v>
       </c>
@@ -1949,7 +2503,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
         <v>1</v>
       </c>
@@ -1987,7 +2541,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
         <v>1</v>
       </c>
@@ -2025,7 +2579,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12" s="41" t="s">
         <v>1</v>
       </c>
@@ -2057,7 +2611,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="2:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -2065,7 +2627,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="2:25" ht="24" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B15" s="8" t="s">
         <v>31</v>
       </c>
@@ -2076,7 +2638,7 @@
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="2:25" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:25" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="E16" s="17"/>
@@ -2088,7 +2650,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="115" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" ht="118.5" x14ac:dyDescent="0.25">
       <c r="B17" s="16" t="s">
         <v>28</v>
       </c>
@@ -2114,7 +2676,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>1</v>
       </c>
@@ -2138,7 +2700,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>1</v>
       </c>
@@ -2162,7 +2724,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>1</v>
       </c>
@@ -2186,8 +2748,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:9" ht="24" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B22" s="8" t="s">
         <v>16</v>
       </c>
@@ -2197,7 +2759,7 @@
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="18" t="s">
@@ -2207,7 +2769,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="2:9" ht="91" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B24" s="16" t="s">
         <v>14</v>
       </c>
@@ -2221,7 +2783,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="12" t="s">
         <v>1</v>
       </c>
@@ -2235,7 +2797,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>1</v>
       </c>
@@ -2249,7 +2811,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
         <v>1</v>
       </c>
@@ -2263,8 +2825,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:9" ht="24" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B29" s="8" t="s">
         <v>8</v>
       </c>
@@ -2274,7 +2836,7 @@
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="31" spans="2:9" ht="130" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:9" ht="131.25" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="s">
         <v>7</v>
       </c>
@@ -2294,7 +2856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>1</v>
       </c>
@@ -2316,31 +2878,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C18">
-    <cfRule type="duplicateValues" dxfId="40" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:D25">
-    <cfRule type="duplicateValues" dxfId="39" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:D27">
-    <cfRule type="duplicateValues" dxfId="38" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:D32">
-    <cfRule type="duplicateValues" dxfId="37" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:C12">
-    <cfRule type="duplicateValues" dxfId="36" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C12">
-    <cfRule type="duplicateValues" dxfId="35" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:C20">
-    <cfRule type="duplicateValues" dxfId="34" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="7"/>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D18:D20" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D18:D20">
       <formula1>"suit, pet, dragon"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E18:E20" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E18:E20">
       <formula1>$C$25:$C$27</formula1>
     </dataValidation>
   </dataValidations>
@@ -2352,4 +2914,524 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F3:M36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4">
+        <f>gacha!E32</f>
+        <v>4</v>
+      </c>
+      <c r="K4" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" s="45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5">
+        <f>gacha!F32</f>
+        <v>0.01</v>
+      </c>
+      <c r="J5" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="49">
+        <v>1</v>
+      </c>
+      <c r="L5" s="49">
+        <v>2</v>
+      </c>
+      <c r="M5" s="49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6">
+        <f>gacha!G32</f>
+        <v>1.4</v>
+      </c>
+      <c r="J6" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="49">
+        <v>1</v>
+      </c>
+      <c r="L6" s="49">
+        <v>2</v>
+      </c>
+      <c r="M6" s="49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="J7" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="49">
+        <v>1</v>
+      </c>
+      <c r="L7" s="49">
+        <v>2</v>
+      </c>
+      <c r="M7" s="49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="J8" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="49">
+        <v>1</v>
+      </c>
+      <c r="L8" s="49">
+        <v>2</v>
+      </c>
+      <c r="M8" s="49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="J9" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="K9" s="42">
+        <v>0</v>
+      </c>
+      <c r="L9" s="42">
+        <v>2</v>
+      </c>
+      <c r="M9" s="42">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="10" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="J10" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="42">
+        <v>0</v>
+      </c>
+      <c r="L10" s="42">
+        <v>0</v>
+      </c>
+      <c r="M10" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="J11" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" s="42">
+        <v>1</v>
+      </c>
+      <c r="L11" s="42">
+        <v>1.5</v>
+      </c>
+      <c r="M11" s="42">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="12" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="K12" s="49">
+        <v>1</v>
+      </c>
+      <c r="L12" s="49">
+        <v>2</v>
+      </c>
+      <c r="M12" s="49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K16" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="L16" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="M16" s="45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J17" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17" s="42">
+        <f>IF(K5=0,0,1/(POWER(K5,$G$4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L17" s="42">
+        <f>IF(L5=0,0,1/(POWER(L5,$G$4)))</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="M17" s="42">
+        <f>IF(M5=0,0,1/(POWER(M5,$G$4)))</f>
+        <v>1.2345679012345678E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J18" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18" s="42">
+        <f t="shared" ref="K18:M24" si="0">IF(K6=0,0,1/(POWER(K6,$G$4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L18" s="42">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="M18" s="42">
+        <f t="shared" si="0"/>
+        <v>1.2345679012345678E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J19" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="K19" s="42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L19" s="42">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="M19" s="42">
+        <f t="shared" si="0"/>
+        <v>1.2345679012345678E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J20" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" s="42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L20" s="42">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="M20" s="42">
+        <f t="shared" si="0"/>
+        <v>1.2345679012345678E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J21" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="K21" s="42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L21" s="42">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="M21" s="42">
+        <f t="shared" si="0"/>
+        <v>4.7958502466985365E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J22" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="K22" s="42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L22" s="42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J23" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="K23" s="42">
+        <f>IF(K11=0,0,1/(POWER(K11,$G$4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L23" s="42">
+        <f t="shared" ref="L23:M24" si="1">IF(L11=0,0,1/(POWER(L11,$G$4)))</f>
+        <v>0.19753086419753085</v>
+      </c>
+      <c r="M23" s="42">
+        <f t="shared" si="1"/>
+        <v>9.5259868922420346E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="10:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J24" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="K24" s="42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L24" s="42">
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="M24" s="42">
+        <f t="shared" si="1"/>
+        <v>1.2345679012345678E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="10:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="10:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K28" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="L28" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="M28" s="45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J29" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="K29" s="50">
+        <f>ROUND(K17/(K17+L17+M17),2)</f>
+        <v>0.93</v>
+      </c>
+      <c r="L29" s="50">
+        <f>ROUND(L17/(K17+L17+M17),2)</f>
+        <v>0.06</v>
+      </c>
+      <c r="M29" s="50">
+        <f>ROUND(M17/(K17+L17+M17),2)</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="30" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J30" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="K30" s="50">
+        <f t="shared" ref="K30:K36" si="2">ROUND(K18/(K18+L18+M18),2)</f>
+        <v>0.93</v>
+      </c>
+      <c r="L30" s="50">
+        <f t="shared" ref="L30:L36" si="3">ROUND(L18/(K18+L18+M18),2)</f>
+        <v>0.06</v>
+      </c>
+      <c r="M30" s="50">
+        <f t="shared" ref="M30:M36" si="4">ROUND(M18/(K18+L18+M18),2)</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="31" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J31" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="K31" s="50">
+        <f t="shared" si="2"/>
+        <v>0.93</v>
+      </c>
+      <c r="L31" s="50">
+        <f t="shared" si="3"/>
+        <v>0.06</v>
+      </c>
+      <c r="M31" s="50">
+        <f t="shared" si="4"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="32" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J32" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="K32" s="50">
+        <f t="shared" si="2"/>
+        <v>0.93</v>
+      </c>
+      <c r="L32" s="50">
+        <f t="shared" si="3"/>
+        <v>0.06</v>
+      </c>
+      <c r="M32" s="50">
+        <f t="shared" si="4"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="33" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J33" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="K33" s="50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L33" s="50">
+        <f t="shared" si="3"/>
+        <v>0.93</v>
+      </c>
+      <c r="M33" s="50">
+        <f t="shared" si="4"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J34" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="K34" s="50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L34" s="50">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M34" s="50">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J35" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="K35" s="50">
+        <f t="shared" si="2"/>
+        <v>0.77</v>
+      </c>
+      <c r="L35" s="50">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
+      </c>
+      <c r="M35" s="50">
+        <f t="shared" si="4"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="10:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J36" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="K36" s="50">
+        <f t="shared" si="2"/>
+        <v>0.93</v>
+      </c>
+      <c r="L36" s="50">
+        <f t="shared" si="3"/>
+        <v>0.06</v>
+      </c>
+      <c r="M36" s="50">
+        <f t="shared" si="4"/>
+        <v>0.01</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="J7:J12">
+    <cfRule type="duplicateValues" dxfId="14" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:J12">
+    <cfRule type="duplicateValues" dxfId="13" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4">
+    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4">
+    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4">
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J19:J24">
+    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17:J24">
+    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L16">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M16">
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J31:J36">
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J29:J36">
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K28">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L28">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M28">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Calculating weights for new egg (egg_BabyGuaranteed)
Former-commit-id: 00e4789186651ff34479c9a3f7a943e52aa4d5bd
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gatcha.xlsx
+++ b/Docs/Content/HungryDragonContent_Gatcha.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="90">
   <si>
     <t>dynamicGatcha</t>
   </si>
@@ -286,6 +286,15 @@
   </si>
   <si>
     <t>DEFAULT PROB NORM</t>
+  </si>
+  <si>
+    <t>new column!</t>
+  </si>
+  <si>
+    <t>[weightBaby]</t>
+  </si>
+  <si>
+    <t>egg_babyGuaranteed</t>
   </si>
 </sst>
 </file>
@@ -620,7 +629,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -710,233 +719,435 @@
     <xf numFmtId="9" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="68">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+  <dxfs count="88">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -947,9 +1158,7 @@
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
+        <right/>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -961,41 +1170,17 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
+        <right/>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -1004,387 +1189,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1403,7 +1207,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1418,7 +1221,190 @@
         <top style="thin">
           <color auto="1"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -1439,14 +1425,13 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
           <color auto="1"/>
@@ -1454,7 +1439,506 @@
         <top style="thin">
           <color auto="1"/>
         </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1473,6 +1957,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1487,9 +1972,7 @@
         <top style="thin">
           <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1508,13 +1991,14 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
           <color auto="1"/>
@@ -1523,91 +2007,6 @@
           <color auto="1"/>
         </top>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -1634,7 +2033,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color auto="1"/>
@@ -1642,192 +2041,7 @@
         <top style="thin">
           <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1852,7 +2066,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color auto="1"/>
@@ -1863,8 +2077,6 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1924,51 +2136,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="eggDefinitions5" displayName="eggDefinitions5" ref="B4:M12" totalsRowShown="0" headerRowDxfId="49" headerRowBorderDxfId="47" tableBorderDxfId="48" totalsRowBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="eggDefinitions5" displayName="eggDefinitions5" ref="B4:M12" totalsRowShown="0" headerRowDxfId="87" headerRowBorderDxfId="86" tableBorderDxfId="85" totalsRowBorderDxfId="84">
   <autoFilter ref="B4:M12"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{eggDefinitions}" dataDxfId="44" totalsRowDxfId="45"/>
-    <tableColumn id="6" name="[sku]" dataDxfId="42" totalsRowDxfId="43"/>
-    <tableColumn id="4" name="[pricePC]" dataDxfId="40" totalsRowDxfId="41"/>
-    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="38" totalsRowDxfId="39"/>
-    <tableColumn id="8" name="[weightCommon]" dataDxfId="36" totalsRowDxfId="37"/>
-    <tableColumn id="9" name="[weightRare]" dataDxfId="34" totalsRowDxfId="35"/>
-    <tableColumn id="11" name="[weightEpic]" dataDxfId="32" totalsRowDxfId="33"/>
-    <tableColumn id="10" name="[prefabPath]" dataDxfId="30" totalsRowDxfId="31"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="28" totalsRowDxfId="29"/>
-    <tableColumn id="12" name="[tidDesc]" dataDxfId="26" totalsRowDxfId="27"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="24" totalsRowDxfId="25"/>
-    <tableColumn id="3" name="[trackingSku]" dataDxfId="22" totalsRowDxfId="23"/>
+    <tableColumn id="1" name="{eggDefinitions}" dataDxfId="83" totalsRowDxfId="82"/>
+    <tableColumn id="6" name="[sku]" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="4" name="[pricePC]" dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="77" totalsRowDxfId="76"/>
+    <tableColumn id="8" name="[weightCommon]" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="9" name="[weightRare]" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="11" name="[weightEpic]" dataDxfId="71" totalsRowDxfId="70"/>
+    <tableColumn id="10" name="[prefabPath]" dataDxfId="69" totalsRowDxfId="68"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="12" name="[tidDesc]" dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="3" name="[trackingSku]" dataDxfId="61" totalsRowDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="eggRewardDefinitions6" displayName="eggRewardDefinitions6" ref="B17:I20" totalsRowShown="0" headerRowDxfId="67" headerRowBorderDxfId="66" tableBorderDxfId="65" totalsRowBorderDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="eggRewardDefinitions6" displayName="eggRewardDefinitions6" ref="B17:I20" totalsRowShown="0" headerRowDxfId="59" headerRowBorderDxfId="58" tableBorderDxfId="57" totalsRowBorderDxfId="56">
   <autoFilter ref="B17:I20"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="63"/>
+    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="55"/>
     <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[type]" dataDxfId="62"/>
-    <tableColumn id="6" name="[rarity]" dataDxfId="61"/>
-    <tableColumn id="4" name="[droprate]" dataDxfId="60"/>
-    <tableColumn id="7" name="[duplicateGemsGiven]" dataDxfId="59"/>
-    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="58"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="57"/>
+    <tableColumn id="3" name="[type]" dataDxfId="54"/>
+    <tableColumn id="6" name="[rarity]" dataDxfId="53"/>
+    <tableColumn id="4" name="[droprate]" dataDxfId="52"/>
+    <tableColumn id="7" name="[duplicateGemsGiven]" dataDxfId="51"/>
+    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="50"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="rarityDefinitions7" displayName="rarityDefinitions7" ref="B24:E27" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54" totalsRowBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="rarityDefinitions7" displayName="rarityDefinitions7" ref="B24:E27" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46" totalsRowBorderDxfId="45">
   <autoFilter ref="B24:E27"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="52"/>
+    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="44"/>
     <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[order]" dataDxfId="51"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="50"/>
+    <tableColumn id="3" name="[order]" dataDxfId="43"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2878,25 +3090,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C18">
-    <cfRule type="duplicateValues" dxfId="21" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:D25">
-    <cfRule type="duplicateValues" dxfId="20" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:D27">
-    <cfRule type="duplicateValues" dxfId="19" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:D32">
-    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:C12">
-    <cfRule type="duplicateValues" dxfId="17" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C12">
-    <cfRule type="duplicateValues" dxfId="16" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:C20">
-    <cfRule type="duplicateValues" dxfId="15" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="7"/>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D18:D20">
@@ -2918,10 +3130,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F3:M36"/>
+  <dimension ref="F3:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2930,14 +3142,18 @@
     <col min="11" max="11" width="18.42578125" customWidth="1"/>
     <col min="12" max="12" width="17.7109375" customWidth="1"/>
     <col min="13" max="13" width="18" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="4" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F4" t="s">
         <v>82</v>
       </c>
@@ -2951,11 +3167,14 @@
       <c r="L4" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="M4" s="45" t="s">
+      <c r="M4" s="44" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="N4" s="45" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>83</v>
       </c>
@@ -2966,17 +3185,20 @@
       <c r="J5" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="49">
+      <c r="K5" s="51">
         <v>1</v>
       </c>
-      <c r="L5" s="49">
+      <c r="L5" s="51">
         <v>2</v>
       </c>
-      <c r="M5" s="49">
+      <c r="M5" s="51">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>84</v>
       </c>
@@ -2996,8 +3218,11 @@
       <c r="M6" s="49">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="6:14" x14ac:dyDescent="0.25">
       <c r="J7" s="47" t="s">
         <v>32</v>
       </c>
@@ -3010,8 +3235,11 @@
       <c r="M7" s="49">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="6:14" x14ac:dyDescent="0.25">
       <c r="J8" s="47" t="s">
         <v>36</v>
       </c>
@@ -3024,8 +3252,11 @@
       <c r="M8" s="49">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="6:14" x14ac:dyDescent="0.25">
       <c r="J9" s="47" t="s">
         <v>49</v>
       </c>
@@ -3038,8 +3269,11 @@
       <c r="M9" s="42">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="10" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="6:14" x14ac:dyDescent="0.25">
       <c r="J10" s="47" t="s">
         <v>50</v>
       </c>
@@ -3050,10 +3284,13 @@
         <v>0</v>
       </c>
       <c r="M10" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="6:13" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="N10" s="42">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="11" spans="6:14" x14ac:dyDescent="0.25">
       <c r="J11" s="47" t="s">
         <v>51</v>
       </c>
@@ -3066,9 +3303,12 @@
       <c r="M11" s="42">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="12" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J12" s="48" t="s">
+      <c r="N11" s="42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="J12" s="47" t="s">
         <v>70</v>
       </c>
       <c r="K12" s="49">
@@ -3080,355 +3320,496 @@
       <c r="M12" s="49">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J15" t="s">
+      <c r="N12" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J13" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="K13" s="42">
+        <v>0</v>
+      </c>
+      <c r="L13" s="42">
+        <v>0</v>
+      </c>
+      <c r="M13" s="42">
+        <v>0</v>
+      </c>
+      <c r="N13" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J16" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K16" s="43" t="s">
+    <row r="17" spans="10:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K17" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="L16" s="44" t="s">
+      <c r="L17" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="M16" s="45" t="s">
+      <c r="M17" s="44" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J17" s="46" t="s">
+      <c r="N17" s="45" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J18" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="K17" s="42">
+      <c r="K18" s="42">
         <f>IF(K5=0,0,1/(POWER(K5,$G$4)))</f>
         <v>1</v>
       </c>
-      <c r="L17" s="42">
+      <c r="L18" s="42">
         <f>IF(L5=0,0,1/(POWER(L5,$G$4)))</f>
         <v>6.25E-2</v>
       </c>
-      <c r="M17" s="42">
+      <c r="M18" s="42">
         <f>IF(M5=0,0,1/(POWER(M5,$G$4)))</f>
         <v>1.2345679012345678E-2</v>
       </c>
-    </row>
-    <row r="18" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J18" s="47" t="s">
+      <c r="N18" s="51">
+        <f>IF(N5=0,0,1/(POWER(N5,$G$4)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J19" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="K18" s="42">
-        <f t="shared" ref="K18:M24" si="0">IF(K6=0,0,1/(POWER(K6,$G$4)))</f>
+      <c r="K19" s="42">
+        <f>IF(K6=0,0,1/(POWER(K6,$G$4)))</f>
         <v>1</v>
       </c>
-      <c r="L18" s="42">
+      <c r="L19" s="42">
+        <f>IF(L6=0,0,1/(POWER(L6,$G$4)))</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="M19" s="42">
+        <f>IF(M6=0,0,1/(POWER(M6,$G$4)))</f>
+        <v>1.2345679012345678E-2</v>
+      </c>
+      <c r="N19" s="51">
+        <f t="shared" ref="N19:N26" si="0">IF(N6=0,0,1/(POWER(N6,$G$4)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J20" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" s="42">
+        <f>IF(K7=0,0,1/(POWER(K7,$G$4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L20" s="42">
+        <f>IF(L7=0,0,1/(POWER(L7,$G$4)))</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="M20" s="42">
+        <f>IF(M7=0,0,1/(POWER(M7,$G$4)))</f>
+        <v>1.2345679012345678E-2</v>
+      </c>
+      <c r="N20" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J21" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="K21" s="42">
+        <f>IF(K8=0,0,1/(POWER(K8,$G$4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L21" s="42">
+        <f>IF(L8=0,0,1/(POWER(L8,$G$4)))</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="M21" s="42">
+        <f>IF(M8=0,0,1/(POWER(M8,$G$4)))</f>
+        <v>1.2345679012345678E-2</v>
+      </c>
+      <c r="N21" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J22" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="K22" s="42">
+        <f>IF(K9=0,0,1/(POWER(K9,$G$4)))</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="42">
+        <f>IF(L9=0,0,1/(POWER(L9,$G$4)))</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="M22" s="42">
+        <f>IF(M9=0,0,1/(POWER(M9,$G$4)))</f>
+        <v>4.7958502466985365E-3</v>
+      </c>
+      <c r="N22" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J23" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="K23" s="42">
+        <f>IF(K10=0,0,1/(POWER(K10,$G$4)))</f>
+        <v>0</v>
+      </c>
+      <c r="L23" s="42">
+        <f>IF(L10=0,0,1/(POWER(L10,$G$4)))</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="42">
+        <f>IF(M10=0,0,1/(POWER(M10,$G$4)))</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="N23" s="51">
+        <f t="shared" si="0"/>
+        <v>4.7958502466985365E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J24" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="K24" s="42">
+        <f>IF(K11=0,0,1/(POWER(K11,$G$4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L24" s="42">
+        <f>IF(L11=0,0,1/(POWER(L11,$G$4)))</f>
+        <v>0.19753086419753085</v>
+      </c>
+      <c r="M24" s="42">
+        <f>IF(M11=0,0,1/(POWER(M11,$G$4)))</f>
+        <v>9.5259868922420346E-2</v>
+      </c>
+      <c r="N24" s="51">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="M18" s="42">
+    </row>
+    <row r="25" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J25" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="K25" s="42">
+        <f>IF(K12=0,0,1/(POWER(K12,$G$4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L25" s="42">
+        <f>IF(L12=0,0,1/(POWER(L12,$G$4)))</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="M25" s="42">
+        <f>IF(M12=0,0,1/(POWER(M12,$G$4)))</f>
+        <v>1.2345679012345678E-2</v>
+      </c>
+      <c r="N25" s="51">
         <f t="shared" si="0"/>
-        <v>1.2345679012345678E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J19" s="47" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="10:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J26" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="K26" s="42">
+        <f>IF(K13=0,0,1/(POWER(K13,$G$4)))</f>
+        <v>0</v>
+      </c>
+      <c r="L26" s="42">
+        <f>IF(L13=0,0,1/(POWER(L13,$G$4)))</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="42">
+        <f>IF(M13=0,0,1/(POWER(M13,$G$4)))</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="51">
+        <f>IF(N13=0,0,1/(POWER(N13,$G$4)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="10:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="10:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K30" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="L30" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="M30" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="N30" s="45" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J31" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="K31" s="50">
+        <f>ROUND(K18/(K18+L18+M18+N18),2)</f>
+        <v>0.93</v>
+      </c>
+      <c r="L31" s="50">
+        <f>ROUND(L18/(K18+L18+M18+N18),2)</f>
+        <v>0.06</v>
+      </c>
+      <c r="M31" s="50">
+        <f>ROUND(M18/(K18+L18+M18+N18),2)</f>
+        <v>0.01</v>
+      </c>
+      <c r="N31" s="50">
+        <f>ROUND(N18/(K18+L18+M18+N18),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J32" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="K32" s="50">
+        <f t="shared" ref="K32:K39" si="1">ROUND(K19/(K19+L19+M19+N19),2)</f>
+        <v>0.93</v>
+      </c>
+      <c r="L32" s="50">
+        <f t="shared" ref="L32:L39" si="2">ROUND(L19/(K19+L19+M19+N19),2)</f>
+        <v>0.06</v>
+      </c>
+      <c r="M32" s="50">
+        <f t="shared" ref="M32:M39" si="3">ROUND(M19/(K19+L19+M19+N19),2)</f>
+        <v>0.01</v>
+      </c>
+      <c r="N32" s="50">
+        <f t="shared" ref="N32:N39" si="4">ROUND(N19/(K19+L19+M19+N19),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J33" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="K19" s="42">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L19" s="42">
-        <f t="shared" si="0"/>
-        <v>6.25E-2</v>
-      </c>
-      <c r="M19" s="42">
-        <f t="shared" si="0"/>
-        <v>1.2345679012345678E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J20" s="47" t="s">
+      <c r="K33" s="50">
+        <f t="shared" si="1"/>
+        <v>0.93</v>
+      </c>
+      <c r="L33" s="50">
+        <f t="shared" si="2"/>
+        <v>0.06</v>
+      </c>
+      <c r="M33" s="50">
+        <f t="shared" si="3"/>
+        <v>0.01</v>
+      </c>
+      <c r="N33" s="50">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J34" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="K20" s="42">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L20" s="42">
-        <f t="shared" si="0"/>
-        <v>6.25E-2</v>
-      </c>
-      <c r="M20" s="42">
-        <f t="shared" si="0"/>
-        <v>1.2345679012345678E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J21" s="47" t="s">
+      <c r="K34" s="50">
+        <f t="shared" si="1"/>
+        <v>0.93</v>
+      </c>
+      <c r="L34" s="50">
+        <f t="shared" si="2"/>
+        <v>0.06</v>
+      </c>
+      <c r="M34" s="50">
+        <f t="shared" si="3"/>
+        <v>0.01</v>
+      </c>
+      <c r="N34" s="50">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J35" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="K21" s="42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L21" s="42">
-        <f t="shared" si="0"/>
-        <v>6.25E-2</v>
-      </c>
-      <c r="M21" s="42">
-        <f t="shared" si="0"/>
-        <v>4.7958502466985365E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J22" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="K22" s="42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L22" s="42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M22" s="42">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J23" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="K23" s="42">
-        <f>IF(K11=0,0,1/(POWER(K11,$G$4)))</f>
-        <v>1</v>
-      </c>
-      <c r="L23" s="42">
-        <f t="shared" ref="L23:M24" si="1">IF(L11=0,0,1/(POWER(L11,$G$4)))</f>
-        <v>0.19753086419753085</v>
-      </c>
-      <c r="M23" s="42">
+      <c r="K35" s="50">
         <f t="shared" si="1"/>
-        <v>9.5259868922420346E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="10:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J24" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="K24" s="42">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L24" s="42">
-        <f t="shared" si="1"/>
-        <v>6.25E-2</v>
-      </c>
-      <c r="M24" s="42">
-        <f t="shared" si="1"/>
-        <v>1.2345679012345678E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="10:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J27" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="10:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K28" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="L28" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="M28" s="45" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J29" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="K29" s="50">
-        <f>ROUND(K17/(K17+L17+M17),2)</f>
-        <v>0.93</v>
-      </c>
-      <c r="L29" s="50">
-        <f>ROUND(L17/(K17+L17+M17),2)</f>
-        <v>0.06</v>
-      </c>
-      <c r="M29" s="50">
-        <f>ROUND(M17/(K17+L17+M17),2)</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="30" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J30" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="K30" s="50">
-        <f t="shared" ref="K30:K36" si="2">ROUND(K18/(K18+L18+M18),2)</f>
-        <v>0.93</v>
-      </c>
-      <c r="L30" s="50">
-        <f t="shared" ref="L30:L36" si="3">ROUND(L18/(K18+L18+M18),2)</f>
-        <v>0.06</v>
-      </c>
-      <c r="M30" s="50">
-        <f t="shared" ref="M30:M36" si="4">ROUND(M18/(K18+L18+M18),2)</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="31" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J31" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="K31" s="50">
+        <v>0</v>
+      </c>
+      <c r="L35" s="50">
         <f t="shared" si="2"/>
         <v>0.93</v>
       </c>
-      <c r="L31" s="50">
+      <c r="M35" s="50">
         <f t="shared" si="3"/>
-        <v>0.06</v>
-      </c>
-      <c r="M31" s="50">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N35" s="50">
         <f t="shared" si="4"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="32" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J32" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="K32" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J36" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="K36" s="50">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="50">
         <f t="shared" si="2"/>
-        <v>0.93</v>
-      </c>
-      <c r="L32" s="50">
-        <f t="shared" si="3"/>
-        <v>0.06</v>
-      </c>
-      <c r="M32" s="50">
-        <f t="shared" si="4"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="33" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J33" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="K33" s="50">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L33" s="50">
+        <v>0</v>
+      </c>
+      <c r="M36" s="50">
         <f t="shared" si="3"/>
         <v>0.93</v>
       </c>
-      <c r="M33" s="50">
+      <c r="N36" s="50">
         <f t="shared" si="4"/>
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="34" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J34" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="K34" s="50">
+    <row r="37" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J37" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="K37" s="50">
+        <f t="shared" si="1"/>
+        <v>0.74</v>
+      </c>
+      <c r="L37" s="50">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L34" s="50">
+        <v>0.15</v>
+      </c>
+      <c r="M37" s="50">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M34" s="50">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N37" s="50">
+        <f t="shared" si="4"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="38" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J38" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="K38" s="50">
+        <f t="shared" si="1"/>
+        <v>0.93</v>
+      </c>
+      <c r="L38" s="50">
+        <f t="shared" si="2"/>
+        <v>0.06</v>
+      </c>
+      <c r="M38" s="50">
+        <f t="shared" si="3"/>
+        <v>0.01</v>
+      </c>
+      <c r="N38" s="50">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="10:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J39" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="K39" s="50">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L39" s="50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M39" s="50">
+        <f>ROUND(M26/(K26+L26+M26+N26),2)</f>
+        <v>0</v>
+      </c>
+      <c r="N39" s="50">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J35" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="K35" s="50">
-        <f t="shared" si="2"/>
-        <v>0.77</v>
-      </c>
-      <c r="L35" s="50">
-        <f t="shared" si="3"/>
-        <v>0.15</v>
-      </c>
-      <c r="M35" s="50">
-        <f t="shared" si="4"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="10:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J36" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="K36" s="50">
-        <f t="shared" si="2"/>
-        <v>0.93</v>
-      </c>
-      <c r="L36" s="50">
-        <f t="shared" si="3"/>
-        <v>0.06</v>
-      </c>
-      <c r="M36" s="50">
-        <f t="shared" si="4"/>
-        <v>0.01</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="J7:J12">
-    <cfRule type="duplicateValues" dxfId="14" priority="14"/>
+  <conditionalFormatting sqref="J7:J13">
+    <cfRule type="duplicateValues" dxfId="34" priority="34"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J5:J12">
-    <cfRule type="duplicateValues" dxfId="13" priority="15"/>
+  <conditionalFormatting sqref="J5:J13">
+    <cfRule type="duplicateValues" dxfId="33" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4">
-    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="32"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N4">
+    <cfRule type="duplicateValues" dxfId="19" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4">
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J19:J24">
+  <conditionalFormatting sqref="J20:J26">
+    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J18:J26">
+    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J33:J39">
     <cfRule type="duplicateValues" dxfId="9" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J17:J24">
+  <conditionalFormatting sqref="J31:J39">
     <cfRule type="duplicateValues" dxfId="8" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K16">
+  <conditionalFormatting sqref="K17">
     <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L16">
+  <conditionalFormatting sqref="L17">
     <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M16">
+  <conditionalFormatting sqref="N17">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J31:J36">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  <conditionalFormatting sqref="M17">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J29:J36">
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+  <conditionalFormatting sqref="K30">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K28">
+  <conditionalFormatting sqref="L30">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L28">
+  <conditionalFormatting sqref="N30">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M28">
+  <conditionalFormatting sqref="M30">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding data to gatcha system to have new rarity, egg and pet
Former-commit-id: 80b3c21ca363e282fa1a002874ad94242b14d2a4
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gatcha.xlsx
+++ b/Docs/Content/HungryDragonContent_Gatcha.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="21360" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="28800" windowHeight="21360"/>
   </bookViews>
   <sheets>
     <sheet name="gacha" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="90">
   <si>
     <t>dynamicGatcha</t>
   </si>
@@ -192,15 +192,6 @@
     <t>[weightEpic]</t>
   </si>
   <si>
-    <t>1.5</t>
-  </si>
-  <si>
-    <t>1.8</t>
-  </si>
-  <si>
-    <t>3.8</t>
-  </si>
-  <si>
     <t>PF_EggBetterRates</t>
   </si>
   <si>
@@ -295,6 +286,15 @@
   </si>
   <si>
     <t>egg_babyGuaranteed</t>
+  </si>
+  <si>
+    <t>egg_baby</t>
+  </si>
+  <si>
+    <t>pet_baby</t>
+  </si>
+  <si>
+    <t>baby</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -625,11 +625,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -697,12 +708,6 @@
     <xf numFmtId="49" fontId="2" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -722,11 +727,16 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="88">
+  <dxfs count="79">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1028,114 +1038,130 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1756,9 +1782,7 @@
         <top style="thin">
           <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1781,76 +1805,6 @@
           <color auto="1"/>
         </top>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2136,51 +2090,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="eggDefinitions5" displayName="eggDefinitions5" ref="B4:M12" totalsRowShown="0" headerRowDxfId="87" headerRowBorderDxfId="86" tableBorderDxfId="85" totalsRowBorderDxfId="84">
-  <autoFilter ref="B4:M12"/>
-  <tableColumns count="12">
-    <tableColumn id="1" name="{eggDefinitions}" dataDxfId="83" totalsRowDxfId="82"/>
-    <tableColumn id="6" name="[sku]" dataDxfId="81" totalsRowDxfId="80"/>
-    <tableColumn id="4" name="[pricePC]" dataDxfId="79" totalsRowDxfId="78"/>
-    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="77" totalsRowDxfId="76"/>
-    <tableColumn id="8" name="[weightCommon]" dataDxfId="75" totalsRowDxfId="74"/>
-    <tableColumn id="9" name="[weightRare]" dataDxfId="73" totalsRowDxfId="72"/>
-    <tableColumn id="11" name="[weightEpic]" dataDxfId="71" totalsRowDxfId="70"/>
-    <tableColumn id="10" name="[prefabPath]" dataDxfId="69" totalsRowDxfId="68"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="67" totalsRowDxfId="66"/>
-    <tableColumn id="12" name="[tidDesc]" dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="63" totalsRowDxfId="62"/>
-    <tableColumn id="3" name="[trackingSku]" dataDxfId="61" totalsRowDxfId="60"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="eggDefinitions5" displayName="eggDefinitions5" ref="B4:N13" totalsRowShown="0" headerRowDxfId="78" headerRowBorderDxfId="77" tableBorderDxfId="76" totalsRowBorderDxfId="75">
+  <autoFilter ref="B4:N13"/>
+  <tableColumns count="13">
+    <tableColumn id="1" name="{eggDefinitions}" dataDxfId="74" totalsRowDxfId="73"/>
+    <tableColumn id="6" name="[sku]" dataDxfId="72" totalsRowDxfId="71"/>
+    <tableColumn id="4" name="[pricePC]" dataDxfId="70" totalsRowDxfId="69"/>
+    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="68" totalsRowDxfId="67"/>
+    <tableColumn id="8" name="[weightCommon]" dataDxfId="33" totalsRowDxfId="66"/>
+    <tableColumn id="9" name="[weightRare]" dataDxfId="32" totalsRowDxfId="65"/>
+    <tableColumn id="11" name="[weightEpic]" dataDxfId="31" totalsRowDxfId="64"/>
+    <tableColumn id="13" name="[weightBaby]" dataDxfId="30" totalsRowDxfId="34"/>
+    <tableColumn id="10" name="[prefabPath]" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="12" name="[tidDesc]" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="3" name="[trackingSku]" dataDxfId="55" totalsRowDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="eggRewardDefinitions6" displayName="eggRewardDefinitions6" ref="B17:I20" totalsRowShown="0" headerRowDxfId="59" headerRowBorderDxfId="58" tableBorderDxfId="57" totalsRowBorderDxfId="56">
-  <autoFilter ref="B17:I20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="eggRewardDefinitions6" displayName="eggRewardDefinitions6" ref="B17:I21" totalsRowShown="0" headerRowDxfId="53" headerRowBorderDxfId="52" tableBorderDxfId="51" totalsRowBorderDxfId="50">
+  <autoFilter ref="B17:I21"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="55"/>
+    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="49"/>
     <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[type]" dataDxfId="54"/>
-    <tableColumn id="6" name="[rarity]" dataDxfId="53"/>
-    <tableColumn id="4" name="[droprate]" dataDxfId="52"/>
-    <tableColumn id="7" name="[duplicateGemsGiven]" dataDxfId="51"/>
-    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="50"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="49"/>
+    <tableColumn id="3" name="[type]" dataDxfId="48"/>
+    <tableColumn id="6" name="[rarity]" dataDxfId="47"/>
+    <tableColumn id="4" name="[droprate]" dataDxfId="46"/>
+    <tableColumn id="7" name="[duplicateGemsGiven]" dataDxfId="45"/>
+    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="44"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="rarityDefinitions7" displayName="rarityDefinitions7" ref="B24:E27" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46" totalsRowBorderDxfId="45">
-  <autoFilter ref="B24:E27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="rarityDefinitions7" displayName="rarityDefinitions7" ref="B25:E29" totalsRowShown="0" headerRowDxfId="42" headerRowBorderDxfId="41" tableBorderDxfId="40" totalsRowBorderDxfId="39">
+  <autoFilter ref="B25:E29"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="44"/>
+    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="38"/>
     <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[order]" dataDxfId="43"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="42"/>
+    <tableColumn id="3" name="[order]" dataDxfId="37"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2452,30 +2407,28 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="B1:Y32"/>
+  <dimension ref="B1:Y34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" customWidth="1"/>
+    <col min="7" max="7" width="27.7265625" customWidth="1"/>
+    <col min="8" max="8" width="25.453125" customWidth="1"/>
     <col min="9" max="9" width="38" customWidth="1"/>
     <col min="10" max="10" width="45" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.28515625" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.26953125" customWidth="1"/>
+    <col min="12" max="12" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:25" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:25" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="8" t="s">
         <v>48</v>
       </c>
@@ -2503,7 +2456,7 @@
       <c r="X2" s="8"/>
       <c r="Y2" s="8"/>
     </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
@@ -2511,7 +2464,7 @@
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="2:25" ht="103.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:25" ht="101" x14ac:dyDescent="0.35">
       <c r="B4" s="16" t="s">
         <v>47</v>
       </c>
@@ -2533,23 +2486,26 @@
       <c r="H4" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="37" t="s">
+      <c r="I4" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="J4" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="36" t="s">
+      <c r="K4" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="36" t="s">
-        <v>72</v>
-      </c>
       <c r="L4" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="M4" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="M4" s="36" t="s">
+      <c r="N4" s="36" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
@@ -2562,26 +2518,35 @@
       <c r="E5" s="28">
         <v>360</v>
       </c>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="27" t="s">
+      <c r="F5" s="49">
+        <v>1</v>
+      </c>
+      <c r="G5" s="49">
+        <v>2</v>
+      </c>
+      <c r="H5" s="49">
+        <v>3</v>
+      </c>
+      <c r="I5" s="49">
+        <v>0</v>
+      </c>
+      <c r="J5" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="35" t="s">
+      <c r="K5" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="35" t="s">
-        <v>73</v>
-      </c>
       <c r="L5" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="M5" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="M5" s="35" t="s">
+      <c r="N5" s="35" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B6" s="12" t="s">
         <v>1</v>
       </c>
@@ -2594,26 +2559,35 @@
       <c r="E6" s="28">
         <v>0</v>
       </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="27" t="s">
+      <c r="F6" s="47">
+        <v>1</v>
+      </c>
+      <c r="G6" s="47">
+        <v>2</v>
+      </c>
+      <c r="H6" s="47">
+        <v>3</v>
+      </c>
+      <c r="I6" s="47">
+        <v>0</v>
+      </c>
+      <c r="J6" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="35" t="s">
+      <c r="K6" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="35" t="s">
-        <v>74</v>
-      </c>
       <c r="L6" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="M6" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="35" t="s">
+      <c r="N6" s="35" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B7" s="34" t="s">
         <v>1</v>
       </c>
@@ -2626,26 +2600,35 @@
       <c r="E7" s="32">
         <v>0</v>
       </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="31" t="s">
+      <c r="F7" s="47">
+        <v>1</v>
+      </c>
+      <c r="G7" s="47">
+        <v>2</v>
+      </c>
+      <c r="H7" s="47">
+        <v>3</v>
+      </c>
+      <c r="I7" s="47">
+        <v>0</v>
+      </c>
+      <c r="J7" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="30" t="s">
+      <c r="K7" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="30" t="s">
-        <v>74</v>
-      </c>
       <c r="L7" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="M7" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="M7" s="30" t="s">
+      <c r="N7" s="30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B8" s="12" t="s">
         <v>1</v>
       </c>
@@ -2658,26 +2641,35 @@
       <c r="E8" s="28">
         <v>0</v>
       </c>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="27" t="s">
+      <c r="F8" s="47">
+        <v>1</v>
+      </c>
+      <c r="G8" s="47">
+        <v>2</v>
+      </c>
+      <c r="H8" s="47">
+        <v>3</v>
+      </c>
+      <c r="I8" s="47">
+        <v>0</v>
+      </c>
+      <c r="J8" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="K8" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="26" t="s">
-        <v>74</v>
-      </c>
       <c r="L8" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="M8" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="M8" s="26" t="s">
+      <c r="N8" s="26" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B9" s="12" t="s">
         <v>1</v>
       </c>
@@ -2690,32 +2682,35 @@
       <c r="E9" s="28">
         <v>0</v>
       </c>
-      <c r="F9" s="39">
-        <v>0</v>
-      </c>
-      <c r="G9" s="39">
+      <c r="F9" s="40">
+        <v>0</v>
+      </c>
+      <c r="G9" s="40">
         <v>2</v>
       </c>
-      <c r="H9" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="J9" s="26" t="s">
+      <c r="H9" s="40">
+        <v>3.8</v>
+      </c>
+      <c r="I9" s="40">
+        <v>0</v>
+      </c>
+      <c r="J9" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="M9" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="K9" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="L9" s="26" t="s">
+      <c r="N9" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="M9" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B10" s="12" t="s">
         <v>1</v>
       </c>
@@ -2728,32 +2723,35 @@
       <c r="E10" s="28">
         <v>0</v>
       </c>
-      <c r="F10" s="39">
-        <v>0</v>
-      </c>
-      <c r="G10" s="39">
-        <v>0</v>
-      </c>
-      <c r="H10" s="39">
-        <v>1</v>
-      </c>
-      <c r="I10" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="J10" s="26" t="s">
+      <c r="F10" s="40">
+        <v>0</v>
+      </c>
+      <c r="G10" s="40">
+        <v>0</v>
+      </c>
+      <c r="H10" s="40">
+        <v>2</v>
+      </c>
+      <c r="I10" s="40">
+        <v>3.8</v>
+      </c>
+      <c r="J10" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="L10" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="M10" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="K10" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="L10" s="26" t="s">
+      <c r="N10" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="M10" s="26" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B11" s="12" t="s">
         <v>1</v>
       </c>
@@ -2766,72 +2764,109 @@
       <c r="E11" s="28">
         <v>0</v>
       </c>
-      <c r="F11" s="39">
-        <v>1</v>
-      </c>
-      <c r="G11" s="39" t="s">
+      <c r="F11" s="40">
+        <v>1</v>
+      </c>
+      <c r="G11" s="40">
+        <v>1.5</v>
+      </c>
+      <c r="H11" s="40">
+        <v>1.8</v>
+      </c>
+      <c r="I11" s="40">
+        <v>2</v>
+      </c>
+      <c r="J11" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="I11" s="27" t="s">
+      <c r="K11" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="L11" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="M11" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="K11" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="L11" s="26" t="s">
+      <c r="N11" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="M11" s="26" t="s">
+    </row>
+    <row r="12" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B12" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="29" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B12" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>70</v>
-      </c>
       <c r="D12" s="20">
         <v>0</v>
       </c>
       <c r="E12" s="28">
         <v>0</v>
       </c>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="27" t="s">
+      <c r="F12" s="47">
+        <v>1</v>
+      </c>
+      <c r="G12" s="47">
+        <v>2</v>
+      </c>
+      <c r="H12" s="47">
+        <v>3</v>
+      </c>
+      <c r="I12" s="47">
+        <v>0</v>
+      </c>
+      <c r="J12" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="K12" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="K12" s="26" t="s">
-        <v>74</v>
-      </c>
       <c r="L12" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="M12" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="M12" s="26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-    </row>
-    <row r="14" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N12" s="26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B13" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="33">
+        <v>0</v>
+      </c>
+      <c r="E13" s="32">
+        <v>0</v>
+      </c>
+      <c r="F13" s="40">
+        <v>0</v>
+      </c>
+      <c r="G13" s="40">
+        <v>0</v>
+      </c>
+      <c r="H13" s="40">
+        <v>0</v>
+      </c>
+      <c r="I13" s="40">
+        <v>1</v>
+      </c>
+      <c r="J13" s="31"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -2839,7 +2874,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="2:25" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:25" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="8" t="s">
         <v>31</v>
       </c>
@@ -2850,7 +2885,7 @@
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="2:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:25" ht="29" x14ac:dyDescent="0.35">
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="E16" s="17"/>
@@ -2862,7 +2897,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="118.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" ht="115" x14ac:dyDescent="0.35">
       <c r="B17" s="16" t="s">
         <v>28</v>
       </c>
@@ -2879,7 +2914,7 @@
         <v>25</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H17" s="22" t="s">
         <v>24</v>
@@ -2888,7 +2923,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="12" t="s">
         <v>1</v>
       </c>
@@ -2912,7 +2947,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="12" t="s">
         <v>1</v>
       </c>
@@ -2936,7 +2971,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" s="12" t="s">
         <v>1</v>
       </c>
@@ -2960,162 +2995,211 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B22" s="8" t="s">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B21" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="33">
+        <v>4</v>
+      </c>
+      <c r="G21" s="52">
+        <v>20</v>
+      </c>
+      <c r="H21" s="52"/>
+      <c r="I21" s="53"/>
+    </row>
+    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="2:9" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="18" t="s">
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-    </row>
-    <row r="24" spans="2:9" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B24" s="16" t="s">
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+    </row>
+    <row r="25" spans="2:9" ht="91.5" x14ac:dyDescent="0.35">
+      <c r="B25" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C25" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D25" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E25" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="11" t="s">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B26" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="10">
-        <v>0</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="11" t="s">
+      <c r="D26" s="10">
+        <v>0</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B27" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="10">
-        <v>1</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="11" t="s">
+      <c r="D27" s="10">
+        <v>1</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B28" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D28" s="10">
         <v>2</v>
       </c>
-      <c r="E27" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B29" s="8" t="s">
+      <c r="E28" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B29" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="54">
+        <v>3</v>
+      </c>
+      <c r="E29" s="53"/>
+    </row>
+    <row r="30" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="31" spans="2:9" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-    </row>
-    <row r="31" spans="2:9" ht="131.25" x14ac:dyDescent="0.25">
-      <c r="B31" s="7" t="s">
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+    </row>
+    <row r="33" spans="2:7" ht="129.5" x14ac:dyDescent="0.35">
+      <c r="B33" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C33" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E33" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F33" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="G33" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="2">
-        <v>1</v>
-      </c>
-      <c r="E32" s="1">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B34" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1">
         <v>4</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F34" s="1">
         <v>0.01</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G34" s="1">
         <v>1.4</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C18">
-    <cfRule type="duplicateValues" dxfId="41" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25:D25">
-    <cfRule type="duplicateValues" dxfId="40" priority="2"/>
+  <conditionalFormatting sqref="C26:D26">
+    <cfRule type="duplicateValues" dxfId="28" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:D27">
-    <cfRule type="duplicateValues" dxfId="39" priority="3"/>
+  <conditionalFormatting sqref="C27:D28">
+    <cfRule type="duplicateValues" dxfId="27" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C32:D32">
-    <cfRule type="duplicateValues" dxfId="38" priority="1"/>
+  <conditionalFormatting sqref="C34:D34">
+    <cfRule type="duplicateValues" dxfId="26" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:C12">
-    <cfRule type="duplicateValues" dxfId="37" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:C12">
-    <cfRule type="duplicateValues" dxfId="36" priority="6"/>
+  <conditionalFormatting sqref="C5:C13">
+    <cfRule type="duplicateValues" dxfId="24" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:C20">
-    <cfRule type="duplicateValues" dxfId="35" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="12"/>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D18:D20">
+  <conditionalFormatting sqref="C13">
+    <cfRule type="duplicateValues" dxfId="22" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="duplicateValues" dxfId="21" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="duplicateValues" dxfId="20" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="duplicateValues" dxfId="19" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29:D29">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D18:D21">
       <formula1>"suit, pet, dragon"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E18:E20">
-      <formula1>$C$25:$C$27</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E18:E21">
+      <formula1>$C$26:$C$29</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3132,685 +3216,685 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F3:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.453125" customWidth="1"/>
+    <col min="11" max="11" width="18.453125" customWidth="1"/>
+    <col min="12" max="12" width="17.7265625" customWidth="1"/>
     <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="6:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="J3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="6:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4">
+        <f>gacha!E34</f>
+        <v>4</v>
+      </c>
+      <c r="K4" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="N4" s="43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="6:14" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5">
+        <f>gacha!F34</f>
+        <v>0.01</v>
+      </c>
+      <c r="J5" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="49">
+        <v>1</v>
+      </c>
+      <c r="L5" s="49">
+        <v>2</v>
+      </c>
+      <c r="M5" s="49">
+        <v>3</v>
+      </c>
+      <c r="N5" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="6:14" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
         <v>81</v>
       </c>
-      <c r="N3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F4" t="s">
+      <c r="G6">
+        <f>gacha!G34</f>
+        <v>1.4</v>
+      </c>
+      <c r="J6" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="47">
+        <v>1</v>
+      </c>
+      <c r="L6" s="47">
+        <v>2</v>
+      </c>
+      <c r="M6" s="47">
+        <v>3</v>
+      </c>
+      <c r="N6" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="6:14" x14ac:dyDescent="0.35">
+      <c r="J7" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="47">
+        <v>1</v>
+      </c>
+      <c r="L7" s="47">
+        <v>2</v>
+      </c>
+      <c r="M7" s="47">
+        <v>3</v>
+      </c>
+      <c r="N7" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="6:14" x14ac:dyDescent="0.35">
+      <c r="J8" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="47">
+        <v>1</v>
+      </c>
+      <c r="L8" s="47">
+        <v>2</v>
+      </c>
+      <c r="M8" s="47">
+        <v>3</v>
+      </c>
+      <c r="N8" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="6:14" x14ac:dyDescent="0.35">
+      <c r="J9" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="K9" s="40">
+        <v>0</v>
+      </c>
+      <c r="L9" s="40">
+        <v>2</v>
+      </c>
+      <c r="M9" s="40">
+        <v>3.8</v>
+      </c>
+      <c r="N9" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="6:14" x14ac:dyDescent="0.35">
+      <c r="J10" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="40">
+        <v>0</v>
+      </c>
+      <c r="L10" s="40">
+        <v>0</v>
+      </c>
+      <c r="M10" s="40">
+        <v>2</v>
+      </c>
+      <c r="N10" s="40">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="11" spans="6:14" x14ac:dyDescent="0.35">
+      <c r="J11" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" s="40">
+        <v>1</v>
+      </c>
+      <c r="L11" s="40">
+        <v>1.5</v>
+      </c>
+      <c r="M11" s="40">
+        <v>1.8</v>
+      </c>
+      <c r="N11" s="40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="6:14" x14ac:dyDescent="0.35">
+      <c r="J12" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" s="47">
+        <v>1</v>
+      </c>
+      <c r="L12" s="47">
+        <v>2</v>
+      </c>
+      <c r="M12" s="47">
+        <v>3</v>
+      </c>
+      <c r="N12" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="6:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J13" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="K13" s="40">
+        <v>0</v>
+      </c>
+      <c r="L13" s="40">
+        <v>0</v>
+      </c>
+      <c r="M13" s="40">
+        <v>0</v>
+      </c>
+      <c r="N13" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="6:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J16" t="s">
         <v>82</v>
       </c>
-      <c r="G4">
-        <f>gacha!E32</f>
-        <v>4</v>
-      </c>
-      <c r="K4" s="43" t="s">
+    </row>
+    <row r="17" spans="10:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K17" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="L4" s="44" t="s">
+      <c r="L17" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="M4" s="44" t="s">
+      <c r="M17" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="N4" s="45" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G5">
-        <f>gacha!F32</f>
-        <v>0.01</v>
-      </c>
-      <c r="J5" s="46" t="s">
+      <c r="N17" s="43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J18" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="51">
-        <v>1</v>
-      </c>
-      <c r="L5" s="51">
-        <v>2</v>
-      </c>
-      <c r="M5" s="51">
-        <v>3</v>
-      </c>
-      <c r="N5" s="51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G6">
-        <f>gacha!G32</f>
-        <v>1.4</v>
-      </c>
-      <c r="J6" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" s="49">
-        <v>1</v>
-      </c>
-      <c r="L6" s="49">
-        <v>2</v>
-      </c>
-      <c r="M6" s="49">
-        <v>3</v>
-      </c>
-      <c r="N6" s="49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="J7" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="49">
-        <v>1</v>
-      </c>
-      <c r="L7" s="49">
-        <v>2</v>
-      </c>
-      <c r="M7" s="49">
-        <v>3</v>
-      </c>
-      <c r="N7" s="49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="J8" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="K8" s="49">
-        <v>1</v>
-      </c>
-      <c r="L8" s="49">
-        <v>2</v>
-      </c>
-      <c r="M8" s="49">
-        <v>3</v>
-      </c>
-      <c r="N8" s="49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="J9" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="K9" s="42">
-        <v>0</v>
-      </c>
-      <c r="L9" s="42">
-        <v>2</v>
-      </c>
-      <c r="M9" s="42">
-        <v>3.8</v>
-      </c>
-      <c r="N9" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="J10" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="K10" s="42">
-        <v>0</v>
-      </c>
-      <c r="L10" s="42">
-        <v>0</v>
-      </c>
-      <c r="M10" s="42">
-        <v>2</v>
-      </c>
-      <c r="N10" s="42">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="11" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="J11" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="K11" s="42">
-        <v>1</v>
-      </c>
-      <c r="L11" s="42">
-        <v>1.5</v>
-      </c>
-      <c r="M11" s="42">
-        <v>1.8</v>
-      </c>
-      <c r="N11" s="42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="J12" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="K12" s="49">
-        <v>1</v>
-      </c>
-      <c r="L12" s="49">
-        <v>2</v>
-      </c>
-      <c r="M12" s="49">
-        <v>3</v>
-      </c>
-      <c r="N12" s="49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J13" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="K13" s="42">
-        <v>0</v>
-      </c>
-      <c r="L13" s="42">
-        <v>0</v>
-      </c>
-      <c r="M13" s="42">
-        <v>0</v>
-      </c>
-      <c r="N13" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="10:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K17" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="L17" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="M17" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="N17" s="45" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J18" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="K18" s="42">
+      <c r="K18" s="40">
         <f>IF(K5=0,0,1/(POWER(K5,$G$4)))</f>
         <v>1</v>
       </c>
-      <c r="L18" s="42">
+      <c r="L18" s="40">
         <f>IF(L5=0,0,1/(POWER(L5,$G$4)))</f>
         <v>6.25E-2</v>
       </c>
-      <c r="M18" s="42">
+      <c r="M18" s="40">
         <f>IF(M5=0,0,1/(POWER(M5,$G$4)))</f>
         <v>1.2345679012345678E-2</v>
       </c>
-      <c r="N18" s="51">
+      <c r="N18" s="49">
         <f>IF(N5=0,0,1/(POWER(N5,$G$4)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J19" s="47" t="s">
+    <row r="19" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J19" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="K19" s="42">
-        <f>IF(K6=0,0,1/(POWER(K6,$G$4)))</f>
-        <v>1</v>
-      </c>
-      <c r="L19" s="42">
-        <f>IF(L6=0,0,1/(POWER(L6,$G$4)))</f>
+      <c r="K19" s="40">
+        <f t="shared" ref="K19:M26" si="0">IF(K6=0,0,1/(POWER(K6,$G$4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L19" s="40">
+        <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="M19" s="42">
-        <f>IF(M6=0,0,1/(POWER(M6,$G$4)))</f>
+      <c r="M19" s="40">
+        <f t="shared" si="0"/>
         <v>1.2345679012345678E-2</v>
       </c>
-      <c r="N19" s="51">
-        <f t="shared" ref="N19:N26" si="0">IF(N6=0,0,1/(POWER(N6,$G$4)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J20" s="47" t="s">
+      <c r="N19" s="49">
+        <f t="shared" ref="N19:N25" si="1">IF(N6=0,0,1/(POWER(N6,$G$4)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J20" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="K20" s="42">
-        <f>IF(K7=0,0,1/(POWER(K7,$G$4)))</f>
-        <v>1</v>
-      </c>
-      <c r="L20" s="42">
-        <f>IF(L7=0,0,1/(POWER(L7,$G$4)))</f>
+      <c r="K20" s="40">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L20" s="40">
+        <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="M20" s="42">
-        <f>IF(M7=0,0,1/(POWER(M7,$G$4)))</f>
+      <c r="M20" s="40">
+        <f t="shared" si="0"/>
         <v>1.2345679012345678E-2</v>
       </c>
-      <c r="N20" s="51">
+      <c r="N20" s="49">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J21" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="K21" s="40">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J21" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="K21" s="42">
-        <f>IF(K8=0,0,1/(POWER(K8,$G$4)))</f>
-        <v>1</v>
-      </c>
-      <c r="L21" s="42">
-        <f>IF(L8=0,0,1/(POWER(L8,$G$4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L21" s="40">
+        <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="M21" s="42">
-        <f>IF(M8=0,0,1/(POWER(M8,$G$4)))</f>
+      <c r="M21" s="40">
+        <f t="shared" si="0"/>
         <v>1.2345679012345678E-2</v>
       </c>
-      <c r="N21" s="51">
+      <c r="N21" s="49">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J22" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="K22" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J22" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="K22" s="42">
-        <f>IF(K9=0,0,1/(POWER(K9,$G$4)))</f>
-        <v>0</v>
-      </c>
-      <c r="L22" s="42">
-        <f>IF(L9=0,0,1/(POWER(L9,$G$4)))</f>
+      <c r="L22" s="40">
+        <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="M22" s="42">
-        <f>IF(M9=0,0,1/(POWER(M9,$G$4)))</f>
-        <v>4.7958502466985365E-3</v>
-      </c>
-      <c r="N22" s="51">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J23" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="K23" s="42">
-        <f>IF(K10=0,0,1/(POWER(K10,$G$4)))</f>
-        <v>0</v>
-      </c>
-      <c r="L23" s="42">
-        <f>IF(L10=0,0,1/(POWER(L10,$G$4)))</f>
-        <v>0</v>
-      </c>
-      <c r="M23" s="42">
-        <f>IF(M10=0,0,1/(POWER(M10,$G$4)))</f>
-        <v>6.25E-2</v>
-      </c>
-      <c r="N23" s="51">
+      <c r="M22" s="40">
         <f t="shared" si="0"/>
         <v>4.7958502466985365E-3</v>
       </c>
-    </row>
-    <row r="24" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J24" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="K24" s="42">
-        <f>IF(K11=0,0,1/(POWER(K11,$G$4)))</f>
-        <v>1</v>
-      </c>
-      <c r="L24" s="42">
-        <f>IF(L11=0,0,1/(POWER(L11,$G$4)))</f>
-        <v>0.19753086419753085</v>
-      </c>
-      <c r="M24" s="42">
-        <f>IF(M11=0,0,1/(POWER(M11,$G$4)))</f>
-        <v>9.5259868922420346E-2</v>
-      </c>
-      <c r="N24" s="51">
+      <c r="N22" s="49">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J23" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="K23" s="40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="40">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-    </row>
-    <row r="25" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J25" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="K25" s="42">
-        <f>IF(K12=0,0,1/(POWER(K12,$G$4)))</f>
-        <v>1</v>
-      </c>
-      <c r="L25" s="42">
-        <f>IF(L12=0,0,1/(POWER(L12,$G$4)))</f>
+      <c r="N23" s="49">
+        <f t="shared" si="1"/>
+        <v>4.7958502466985365E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J24" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="K24" s="40">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L24" s="40">
+        <f t="shared" si="0"/>
+        <v>0.19753086419753085</v>
+      </c>
+      <c r="M24" s="40">
+        <f t="shared" si="0"/>
+        <v>9.5259868922420346E-2</v>
+      </c>
+      <c r="N24" s="49">
+        <f t="shared" si="1"/>
         <v>6.25E-2</v>
       </c>
-      <c r="M25" s="42">
-        <f>IF(M12=0,0,1/(POWER(M12,$G$4)))</f>
+    </row>
+    <row r="25" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J25" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="K25" s="40">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L25" s="40">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="M25" s="40">
+        <f t="shared" si="0"/>
         <v>1.2345679012345678E-2</v>
       </c>
-      <c r="N25" s="51">
+      <c r="N25" s="49">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="10:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J26" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="K26" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="10:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J26" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="K26" s="42">
-        <f>IF(K13=0,0,1/(POWER(K13,$G$4)))</f>
-        <v>0</v>
-      </c>
-      <c r="L26" s="42">
-        <f>IF(L13=0,0,1/(POWER(L13,$G$4)))</f>
-        <v>0</v>
-      </c>
-      <c r="M26" s="42">
-        <f>IF(M13=0,0,1/(POWER(M13,$G$4)))</f>
-        <v>0</v>
-      </c>
-      <c r="N26" s="51">
+      <c r="L26" s="40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="49">
         <f>IF(N13=0,0,1/(POWER(N13,$G$4)))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="10:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="10:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="J29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="10:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K30" s="43" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="10:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K30" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="L30" s="44" t="s">
+      <c r="L30" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="M30" s="44" t="s">
+      <c r="M30" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="N30" s="45" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J31" s="46" t="s">
+      <c r="N30" s="43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J31" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="K31" s="50">
+      <c r="K31" s="48">
         <f>ROUND(K18/(K18+L18+M18+N18),2)</f>
         <v>0.93</v>
       </c>
-      <c r="L31" s="50">
+      <c r="L31" s="48">
         <f>ROUND(L18/(K18+L18+M18+N18),2)</f>
         <v>0.06</v>
       </c>
-      <c r="M31" s="50">
+      <c r="M31" s="48">
         <f>ROUND(M18/(K18+L18+M18+N18),2)</f>
         <v>0.01</v>
       </c>
-      <c r="N31" s="50">
+      <c r="N31" s="48">
         <f>ROUND(N18/(K18+L18+M18+N18),2)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J32" s="47" t="s">
+    <row r="32" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J32" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="K32" s="50">
-        <f t="shared" ref="K32:K39" si="1">ROUND(K19/(K19+L19+M19+N19),2)</f>
+      <c r="K32" s="48">
+        <f t="shared" ref="K32:K39" si="2">ROUND(K19/(K19+L19+M19+N19),2)</f>
         <v>0.93</v>
       </c>
-      <c r="L32" s="50">
-        <f t="shared" ref="L32:L39" si="2">ROUND(L19/(K19+L19+M19+N19),2)</f>
+      <c r="L32" s="48">
+        <f t="shared" ref="L32:L39" si="3">ROUND(L19/(K19+L19+M19+N19),2)</f>
         <v>0.06</v>
       </c>
-      <c r="M32" s="50">
-        <f t="shared" ref="M32:M39" si="3">ROUND(M19/(K19+L19+M19+N19),2)</f>
+      <c r="M32" s="48">
+        <f t="shared" ref="M32:M38" si="4">ROUND(M19/(K19+L19+M19+N19),2)</f>
         <v>0.01</v>
       </c>
-      <c r="N32" s="50">
-        <f t="shared" ref="N32:N39" si="4">ROUND(N19/(K19+L19+M19+N19),2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J33" s="47" t="s">
+      <c r="N32" s="48">
+        <f t="shared" ref="N32:N39" si="5">ROUND(N19/(K19+L19+M19+N19),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J33" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="K33" s="50">
-        <f t="shared" si="1"/>
-        <v>0.93</v>
-      </c>
-      <c r="L33" s="50">
-        <f t="shared" si="2"/>
-        <v>0.06</v>
-      </c>
-      <c r="M33" s="50">
-        <f t="shared" si="3"/>
-        <v>0.01</v>
-      </c>
-      <c r="N33" s="50">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J34" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="K34" s="50">
-        <f t="shared" si="1"/>
-        <v>0.93</v>
-      </c>
-      <c r="L34" s="50">
-        <f t="shared" si="2"/>
-        <v>0.06</v>
-      </c>
-      <c r="M34" s="50">
-        <f t="shared" si="3"/>
-        <v>0.01</v>
-      </c>
-      <c r="N34" s="50">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J35" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="K35" s="50">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L35" s="50">
+      <c r="K33" s="48">
         <f t="shared" si="2"/>
         <v>0.93</v>
       </c>
-      <c r="M35" s="50">
+      <c r="L33" s="48">
         <f t="shared" si="3"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="N35" s="50">
+        <v>0.06</v>
+      </c>
+      <c r="M33" s="48">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J36" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="K36" s="50">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L36" s="50">
+        <v>0.01</v>
+      </c>
+      <c r="N33" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J34" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="K34" s="48">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M36" s="50">
+        <v>0.93</v>
+      </c>
+      <c r="L34" s="48">
+        <f t="shared" si="3"/>
+        <v>0.06</v>
+      </c>
+      <c r="M34" s="48">
+        <f t="shared" si="4"/>
+        <v>0.01</v>
+      </c>
+      <c r="N34" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J35" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="K35" s="48">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L35" s="48">
         <f t="shared" si="3"/>
         <v>0.93</v>
       </c>
-      <c r="N36" s="50">
+      <c r="M35" s="48">
         <f t="shared" si="4"/>
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="37" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J37" s="47" t="s">
+      <c r="N35" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J36" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="K36" s="48">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="48">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="48">
+        <f t="shared" si="4"/>
+        <v>0.93</v>
+      </c>
+      <c r="N36" s="48">
+        <f t="shared" si="5"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J37" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="K37" s="50">
-        <f t="shared" si="1"/>
+      <c r="K37" s="48">
+        <f t="shared" si="2"/>
         <v>0.74</v>
       </c>
-      <c r="L37" s="50">
+      <c r="L37" s="48">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
+      </c>
+      <c r="M37" s="48">
+        <f t="shared" si="4"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N37" s="48">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="38" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J38" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="K38" s="48">
         <f t="shared" si="2"/>
-        <v>0.15</v>
-      </c>
-      <c r="M37" s="50">
+        <v>0.93</v>
+      </c>
+      <c r="L38" s="48">
         <f t="shared" si="3"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="N37" s="50">
+        <v>0.06</v>
+      </c>
+      <c r="M38" s="48">
         <f t="shared" si="4"/>
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="38" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J38" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="K38" s="50">
-        <f t="shared" si="1"/>
-        <v>0.93</v>
-      </c>
-      <c r="L38" s="50">
+        <v>0.01</v>
+      </c>
+      <c r="N38" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="10:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J39" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="K39" s="48">
         <f t="shared" si="2"/>
-        <v>0.06</v>
-      </c>
-      <c r="M38" s="50">
+        <v>0</v>
+      </c>
+      <c r="L39" s="48">
         <f t="shared" si="3"/>
-        <v>0.01</v>
-      </c>
-      <c r="N38" s="50">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="10:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J39" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="K39" s="50">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L39" s="50">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M39" s="50">
+        <v>0</v>
+      </c>
+      <c r="M39" s="48">
         <f>ROUND(M26/(K26+L26+M26+N26),2)</f>
         <v>0</v>
       </c>
-      <c r="N39" s="50">
-        <f t="shared" si="4"/>
+      <c r="N39" s="48">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J7:J13">
-    <cfRule type="duplicateValues" dxfId="34" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J13">
-    <cfRule type="duplicateValues" dxfId="33" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4">
-    <cfRule type="duplicateValues" dxfId="32" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="duplicateValues" dxfId="31" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="duplicateValues" dxfId="19" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4">
-    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:J26">
-    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:J26">
-    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J33:J39">
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31:J39">
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N30">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M30">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding some comments to the tables
Former-commit-id: 50647f9951591403723835c734581808489c7604
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gatcha.xlsx
+++ b/Docs/Content/HungryDragonContent_Gatcha.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="97">
   <si>
     <t>dynamicGatcha</t>
   </si>
@@ -313,13 +313,16 @@
   </si>
   <si>
     <t>TID_RARITY_BABY</t>
+  </si>
+  <si>
+    <t>NOT USED ANYMORE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,6 +369,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -658,7 +669,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -750,11 +761,90 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="78">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1093,76 +1183,6 @@
           <color auto="1"/>
         </left>
         <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -2126,24 +2146,24 @@
     <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="31"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="3" name="[type]" dataDxfId="30"/>
-    <tableColumn id="6" name="[rarity]" dataDxfId="29"/>
-    <tableColumn id="4" name="[droprate]" dataDxfId="28"/>
-    <tableColumn id="7" name="[duplicateGemsGiven]" dataDxfId="27"/>
-    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="26"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="25"/>
+    <tableColumn id="6" name="[rarity]" dataDxfId="2"/>
+    <tableColumn id="4" name="[droprate]" dataDxfId="0"/>
+    <tableColumn id="7" name="[duplicateGemsGiven]" dataDxfId="1"/>
+    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="29"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="rarityDefinitions7" displayName="rarityDefinitions7" ref="B25:E29" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="rarityDefinitions7" displayName="rarityDefinitions7" ref="B25:E29" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <autoFilter ref="B25:E29"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="20"/>
+    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="23"/>
     <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[order]" dataDxfId="19"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="18"/>
+    <tableColumn id="3" name="[order]" dataDxfId="22"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2417,8 +2437,8 @@
   </sheetPr>
   <dimension ref="B1:Y34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2907,7 +2927,9 @@
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
+      <c r="F16" s="17" t="s">
+        <v>96</v>
+      </c>
       <c r="G16" s="17" t="s">
         <v>30</v>
       </c>
@@ -2928,7 +2950,7 @@
       <c r="E17" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="55" t="s">
         <v>25</v>
       </c>
       <c r="G17" s="22" t="s">
@@ -2954,7 +2976,7 @@
       <c r="E18" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="56">
         <v>1</v>
       </c>
       <c r="G18" s="19"/>
@@ -2978,7 +3000,7 @@
       <c r="E19" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="20">
+      <c r="F19" s="56">
         <v>2</v>
       </c>
       <c r="G19" s="19"/>
@@ -3002,7 +3024,7 @@
       <c r="E20" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="20">
+      <c r="F20" s="56">
         <v>3</v>
       </c>
       <c r="G20" s="19">
@@ -3026,7 +3048,7 @@
       <c r="E21" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F21" s="33">
+      <c r="F21" s="57">
         <v>4</v>
       </c>
       <c r="G21" s="52">
@@ -3865,58 +3887,58 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J7:J13">
-    <cfRule type="duplicateValues" dxfId="17" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J13">
-    <cfRule type="duplicateValues" dxfId="16" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4">
-    <cfRule type="duplicateValues" dxfId="15" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="duplicateValues" dxfId="14" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="duplicateValues" dxfId="13" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4">
-    <cfRule type="duplicateValues" dxfId="12" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:J26">
-    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:J26">
-    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J33:J39">
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31:J39">
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N30">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M30">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Baby egg sku renamed to "egg_babyGuaranteed"
Former-commit-id: 11a1471363520e5431ad9b742a958c98e4daf6d9
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gatcha.xlsx
+++ b/Docs/Content/HungryDragonContent_Gatcha.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcamacho\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2437,8 +2437,8 @@
   </sheetPr>
   <dimension ref="B1:Y34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2868,7 +2868,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D13" s="33">
         <v>0</v>
@@ -3260,8 +3260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F3:N39"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added welcome eggs fixed offer amount reward, enable true Added new eggs to daily welcome back
Former-commit-id: a8c450a21264ceb2619070284aac67c76f515a02
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gatcha.xlsx
+++ b/Docs/Content/HungryDragonContent_Gatcha.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="99">
   <si>
     <t>dynamicGatcha</t>
   </si>
@@ -316,6 +316,12 @@
   </si>
   <si>
     <t>gems given when duplicate</t>
+  </si>
+  <si>
+    <t>egg_dailyLogin_baby_welcomeBack</t>
+  </si>
+  <si>
+    <t>egg_dailyLogin_betterRates_welcomeBack</t>
   </si>
 </sst>
 </file>
@@ -770,7 +776,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="78">
+  <dxfs count="90">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -862,96 +868,7 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -962,7 +879,9 @@
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -974,17 +893,41 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -993,6 +936,441 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1011,6 +1389,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1025,194 +1404,7 @@
         <top style="thin">
           <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
+        <bottom/>
         <vertical/>
         <horizontal/>
       </border>
@@ -1233,13 +1425,14 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color auto="1"/>
@@ -1247,560 +1440,7 @@
         <top style="thin">
           <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1819,7 +1459,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1834,7 +1473,9 @@
         <top style="thin">
           <color auto="1"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1853,14 +1494,13 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color auto="1"/>
@@ -1869,6 +1509,421 @@
           <color auto="1"/>
         </top>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -1895,7 +1950,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
           <color auto="1"/>
@@ -1903,7 +1958,196 @@
         <top style="thin">
           <color auto="1"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1928,7 +2172,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
           <color auto="1"/>
@@ -1939,6 +2183,8 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1983,126 +2229,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2118,52 +2244,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="eggDefinitions5" displayName="eggDefinitions5" ref="B4:N13" totalsRowShown="0" headerRowDxfId="65" headerRowBorderDxfId="64" tableBorderDxfId="63" totalsRowBorderDxfId="62">
-  <autoFilter ref="B4:N13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="eggDefinitions5" displayName="eggDefinitions5" ref="B4:N15" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="36" tableBorderDxfId="37" totalsRowBorderDxfId="35">
+  <autoFilter ref="B4:N15"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="{eggDefinitions}" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="6" name="[sku]" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="4" name="[pricePC]" dataDxfId="57" totalsRowDxfId="56"/>
-    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="55" totalsRowDxfId="54"/>
-    <tableColumn id="8" name="[weightCommon]" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="9" name="[weightRare]" dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="11" name="[weightEpic]" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="13" name="[weightBaby]" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="10" name="[prefabPath]" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="12" name="[tidDesc]" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="2" name="[icon]" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="3" name="[trackingSku]" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="1" name="{eggDefinitions}" dataDxfId="33" totalsRowDxfId="34"/>
+    <tableColumn id="6" name="[sku]" dataDxfId="31" totalsRowDxfId="32"/>
+    <tableColumn id="4" name="[pricePC]" dataDxfId="29" totalsRowDxfId="30"/>
+    <tableColumn id="5" name="[incubationMinutes]" dataDxfId="27" totalsRowDxfId="28"/>
+    <tableColumn id="8" name="[weightCommon]" dataDxfId="25" totalsRowDxfId="26"/>
+    <tableColumn id="9" name="[weightRare]" dataDxfId="23" totalsRowDxfId="24"/>
+    <tableColumn id="11" name="[weightEpic]" dataDxfId="21" totalsRowDxfId="22"/>
+    <tableColumn id="13" name="[weightBaby]" dataDxfId="19" totalsRowDxfId="20"/>
+    <tableColumn id="10" name="[prefabPath]" dataDxfId="17" totalsRowDxfId="18"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="15" totalsRowDxfId="16"/>
+    <tableColumn id="12" name="[tidDesc]" dataDxfId="13" totalsRowDxfId="14"/>
+    <tableColumn id="2" name="[icon]" dataDxfId="11" totalsRowDxfId="12"/>
+    <tableColumn id="3" name="[trackingSku]" dataDxfId="9" totalsRowDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="eggRewardDefinitions6" displayName="eggRewardDefinitions6" ref="B17:I21" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
-  <autoFilter ref="B17:I21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="eggRewardDefinitions6" displayName="eggRewardDefinitions6" ref="B19:I23" totalsRowShown="0" headerRowDxfId="89" headerRowBorderDxfId="88" tableBorderDxfId="87" totalsRowBorderDxfId="86">
+  <autoFilter ref="B19:I23"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="31"/>
+    <tableColumn id="1" name="{eggRewardDefinitions}" dataDxfId="85"/>
     <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[type]" dataDxfId="30"/>
-    <tableColumn id="6" name="[rarity]" dataDxfId="29"/>
-    <tableColumn id="4" name="[droprate]" dataDxfId="28"/>
-    <tableColumn id="7" name="[duplicateGemsGiven]" dataDxfId="27"/>
-    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="26"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="25"/>
+    <tableColumn id="3" name="[type]" dataDxfId="84"/>
+    <tableColumn id="6" name="[rarity]" dataDxfId="83"/>
+    <tableColumn id="4" name="[droprate]" dataDxfId="82"/>
+    <tableColumn id="7" name="[duplicateGemsGiven]" dataDxfId="81"/>
+    <tableColumn id="8" name="[duplicateCoinsGiven]" dataDxfId="80"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="rarityDefinitions7" displayName="rarityDefinitions7" ref="B25:E29" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
-  <autoFilter ref="B25:E29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="rarityDefinitions7" displayName="rarityDefinitions7" ref="B27:E31" totalsRowShown="0" headerRowDxfId="78" headerRowBorderDxfId="77" tableBorderDxfId="76" totalsRowBorderDxfId="75">
+  <autoFilter ref="B27:E31"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="20"/>
+    <tableColumn id="1" name="{rarityDefinitions}" dataDxfId="74"/>
     <tableColumn id="2" name="[sku]"/>
-    <tableColumn id="3" name="[order]" dataDxfId="19"/>
-    <tableColumn id="5" name="[tidName]" dataDxfId="18"/>
+    <tableColumn id="3" name="[order]" dataDxfId="73"/>
+    <tableColumn id="5" name="[tidName]" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2435,10 +2561,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="B1:Y34"/>
+  <dimension ref="B1:Y36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2904,111 +3030,145 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-    </row>
-    <row r="15" spans="2:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="2:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B14" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="20">
+        <v>0</v>
+      </c>
+      <c r="E14" s="28">
+        <v>0</v>
+      </c>
+      <c r="F14" s="40">
+        <v>1</v>
+      </c>
+      <c r="G14" s="40">
+        <v>1.5</v>
+      </c>
+      <c r="H14" s="40">
+        <v>1.8</v>
+      </c>
+      <c r="I14" s="40">
+        <v>2</v>
+      </c>
+      <c r="J14" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="L14" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="M14" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="N14" s="26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B15" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="33">
+        <v>0</v>
+      </c>
+      <c r="E15" s="32">
+        <v>0</v>
+      </c>
+      <c r="F15" s="40">
+        <v>0</v>
+      </c>
+      <c r="G15" s="40">
+        <v>0</v>
+      </c>
+      <c r="H15" s="40">
+        <v>3.8</v>
+      </c>
+      <c r="I15" s="40">
+        <v>2</v>
+      </c>
+      <c r="J15" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="K15" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="L15" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="M15" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="N15" s="30" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="17"/>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G18" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H18" s="18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="118.5" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
+    <row r="19" spans="2:9" ht="118.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C19" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D19" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E19" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="55" t="s">
+      <c r="F19" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="22" t="s">
+      <c r="G19" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="22" t="s">
+      <c r="H19" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="I19" s="13" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="56">
-        <v>1</v>
-      </c>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19">
-        <v>5000</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="56">
-        <v>2</v>
-      </c>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19">
-        <v>10000</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -3016,110 +3176,130 @@
         <v>1</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D20" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F20" s="56">
-        <v>3</v>
-      </c>
-      <c r="G20" s="19">
-        <v>10</v>
-      </c>
-      <c r="H20" s="19"/>
+        <v>1</v>
+      </c>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19">
+        <v>5000</v>
+      </c>
       <c r="I20" s="9" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="51" t="s">
-        <v>87</v>
+      <c r="C21" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="D21" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E21" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="56">
+        <v>2</v>
+      </c>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19">
+        <v>10000</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="56">
+        <v>3</v>
+      </c>
+      <c r="G22" s="19">
+        <v>10</v>
+      </c>
+      <c r="H22" s="19"/>
+      <c r="I22" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="F21" s="57">
+      <c r="F23" s="57">
         <v>4</v>
       </c>
-      <c r="G21" s="52">
+      <c r="G23" s="52">
         <v>15</v>
       </c>
-      <c r="H21" s="52"/>
-      <c r="I21" s="53" t="s">
+      <c r="H23" s="52"/>
+      <c r="I23" s="53" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B23" s="8" t="s">
+    <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B25" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="18" t="s">
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-    </row>
-    <row r="25" spans="2:9" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B25" s="16" t="s">
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+    </row>
+    <row r="27" spans="2:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="B27" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C27" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D27" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E27" s="13" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="10">
-        <v>0</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="10">
-        <v>1</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
@@ -3127,123 +3307,157 @@
         <v>1</v>
       </c>
       <c r="C28" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="10">
+        <v>1</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D30" s="10">
         <v>2</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E30" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="50" t="s">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="51" t="s">
+      <c r="C31" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="D29" s="54">
+      <c r="D31" s="54">
         <v>3</v>
       </c>
-      <c r="E29" s="53" t="s">
+      <c r="E31" s="53" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B31" s="8" t="s">
+    <row r="32" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B33" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-    </row>
-    <row r="33" spans="2:7" ht="131.25" x14ac:dyDescent="0.25">
-      <c r="B33" s="7" t="s">
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+    </row>
+    <row r="35" spans="2:7" ht="131.25" x14ac:dyDescent="0.25">
+      <c r="B35" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C35" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D35" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E35" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F35" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="G35" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34" s="2">
+      <c r="C36" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2">
         <v>1</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E36" s="1">
         <v>4</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F36" s="1">
         <v>0.01</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G36" s="1">
         <v>1.4</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C18">
-    <cfRule type="duplicateValues" dxfId="77" priority="9"/>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="duplicateValues" dxfId="71" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:D26">
-    <cfRule type="duplicateValues" dxfId="76" priority="7"/>
+  <conditionalFormatting sqref="C28:D28">
+    <cfRule type="duplicateValues" dxfId="70" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27:D28">
-    <cfRule type="duplicateValues" dxfId="75" priority="8"/>
+  <conditionalFormatting sqref="C29:D30">
+    <cfRule type="duplicateValues" dxfId="69" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34:D34">
-    <cfRule type="duplicateValues" dxfId="74" priority="6"/>
+  <conditionalFormatting sqref="C36:D36">
+    <cfRule type="duplicateValues" dxfId="68" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:C12">
-    <cfRule type="duplicateValues" dxfId="73" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:C13">
-    <cfRule type="duplicateValues" dxfId="72" priority="11"/>
+  <conditionalFormatting sqref="C5:C15">
+    <cfRule type="duplicateValues" dxfId="8" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19:C20">
-    <cfRule type="duplicateValues" dxfId="71" priority="12"/>
+  <conditionalFormatting sqref="C21:C22">
+    <cfRule type="duplicateValues" dxfId="66" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="duplicateValues" dxfId="70" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="duplicateValues" dxfId="69" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="duplicateValues" dxfId="68" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
-    <cfRule type="duplicateValues" dxfId="67" priority="2"/>
+  <conditionalFormatting sqref="C23">
+    <cfRule type="duplicateValues" dxfId="62" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:D29">
-    <cfRule type="duplicateValues" dxfId="66" priority="1"/>
+  <conditionalFormatting sqref="C31:D31">
+    <cfRule type="duplicateValues" dxfId="61" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:C15">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:C15">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D18:D21">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D20:D23">
       <formula1>"suit, pet, dragon"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E18:E21">
-      <formula1>$C$26:$C$29</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E20:E23">
+      <formula1>$C$28:$C$31</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3286,7 +3500,7 @@
         <v>78</v>
       </c>
       <c r="G4">
-        <f>gacha!E34</f>
+        <f>gacha!E36</f>
         <v>4</v>
       </c>
       <c r="K4" s="41" t="s">
@@ -3307,7 +3521,7 @@
         <v>79</v>
       </c>
       <c r="G5">
-        <f>gacha!F34</f>
+        <f>gacha!F36</f>
         <v>0.01</v>
       </c>
       <c r="J5" s="44" t="s">
@@ -3331,7 +3545,7 @@
         <v>80</v>
       </c>
       <c r="G6">
-        <f>gacha!G34</f>
+        <f>gacha!G36</f>
         <v>1.4</v>
       </c>
       <c r="J6" s="45" t="s">
@@ -3887,58 +4101,58 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J7:J13">
-    <cfRule type="duplicateValues" dxfId="17" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J13">
-    <cfRule type="duplicateValues" dxfId="16" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4">
-    <cfRule type="duplicateValues" dxfId="15" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="duplicateValues" dxfId="14" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="duplicateValues" dxfId="13" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4">
-    <cfRule type="duplicateValues" dxfId="12" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:J26">
-    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:J26">
-    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J33:J39">
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31:J39">
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N30">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M30">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>